<commit_message>
working version up to TP continuity
</commit_message>
<xml_diff>
--- a/Moonfish Batch Lifetime.xlsx
+++ b/Moonfish Batch Lifetime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry.Delalis\PycharmProjects\moonfish_tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A66D49-54CE-4379-B16E-B3D3C242F06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BAB68C-F26B-4ADD-8B36-AA37C90DB66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -878,7 +878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -983,6 +983,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,9 +995,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1026,16 +1026,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1056,20 +1056,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1117,7 +1120,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1162,6 +1165,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1478,7 +1484,7 @@
   <dimension ref="A1:BK53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1492,18 +1498,18 @@
     <col min="16" max="21" width="9.1796875" style="1" customWidth="1"/>
     <col min="22" max="22" width="3.7265625" style="1" customWidth="1"/>
     <col min="23" max="23" width="25.1796875" style="1" customWidth="1"/>
-    <col min="24" max="49" width="9.1796875" style="1" customWidth="1"/>
-    <col min="50" max="16384" width="9.1796875" style="1"/>
+    <col min="24" max="56" width="9.1796875" style="1" customWidth="1"/>
+    <col min="57" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
       <c r="D1" s="65"/>
-      <c r="F1" s="117" t="s">
+      <c r="F1" s="119" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="64"/>
@@ -1511,70 +1517,70 @@
       <c r="I1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="97" t="s">
+      <c r="J1" s="98" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="65"/>
     </row>
     <row r="2" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="93" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="78"/>
-      <c r="F2" s="109" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="94"/>
+      <c r="A2" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="79"/>
+      <c r="F2" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="95"/>
       <c r="H2" s="21"/>
       <c r="I2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="108" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="78"/>
+      <c r="J2" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="79"/>
     </row>
     <row r="3" spans="1:63" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="124" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
       <c r="D3" s="68"/>
-      <c r="F3" s="109" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="94"/>
+      <c r="F3" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="95"/>
       <c r="H3" s="31"/>
       <c r="I3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="108" t="s">
+      <c r="J3" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="78"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="109" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="94"/>
+      <c r="F4" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="95"/>
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="82" t="s">
+      <c r="J4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="78"/>
+      <c r="K4" s="79"/>
       <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="102" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="67"/>
@@ -1584,7 +1590,7 @@
       <c r="I5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="120" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="68"/>
@@ -1615,7 +1621,7 @@
         <v>15</v>
       </c>
       <c r="I7" s="60"/>
-      <c r="J7" s="106" t="s">
+      <c r="J7" s="107" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="60"/>
@@ -1644,14 +1650,14 @@
       <c r="Z7" s="60"/>
       <c r="AA7" s="60"/>
       <c r="AB7" s="60"/>
-      <c r="AC7" s="111" t="s">
+      <c r="AC7" s="112" t="s">
         <v>15</v>
       </c>
       <c r="AD7" s="67"/>
       <c r="AE7" s="67"/>
       <c r="AF7" s="67"/>
       <c r="AG7" s="67"/>
-      <c r="AH7" s="111" t="s">
+      <c r="AH7" s="112" t="s">
         <v>15</v>
       </c>
       <c r="AI7" s="67"/>
@@ -1700,37 +1706,37 @@
       </c>
       <c r="B8" s="70"/>
       <c r="C8" s="70"/>
-      <c r="D8" s="102" t="s">
+      <c r="D8" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="103"/>
-      <c r="F8" s="102" t="s">
+      <c r="E8" s="104"/>
+      <c r="F8" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="103"/>
-      <c r="H8" s="102" t="s">
+      <c r="G8" s="104"/>
+      <c r="H8" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="103"/>
-      <c r="J8" s="102" t="s">
+      <c r="I8" s="104"/>
+      <c r="J8" s="103" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="70"/>
       <c r="L8" s="70"/>
       <c r="M8" s="70"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="102" t="s">
+      <c r="N8" s="104"/>
+      <c r="O8" s="103" t="s">
         <v>21</v>
       </c>
       <c r="P8" s="70"/>
       <c r="Q8" s="70"/>
       <c r="R8" s="70"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="102" t="s">
+      <c r="S8" s="104"/>
+      <c r="T8" s="103" t="s">
         <v>22</v>
       </c>
       <c r="U8" s="70"/>
-      <c r="V8" s="103"/>
+      <c r="V8" s="104"/>
       <c r="W8" s="19" t="s">
         <v>23</v>
       </c>
@@ -1741,16 +1747,16 @@
       <c r="Z8" s="70"/>
       <c r="AA8" s="70"/>
       <c r="AB8" s="70"/>
-      <c r="AC8" s="72"/>
-      <c r="AD8" s="54"/>
-      <c r="AE8" s="54"/>
-      <c r="AF8" s="54"/>
-      <c r="AG8" s="55"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="54"/>
-      <c r="AJ8" s="54"/>
-      <c r="AK8" s="54"/>
-      <c r="AL8" s="55"/>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="57"/>
+      <c r="AE8" s="57"/>
+      <c r="AF8" s="57"/>
+      <c r="AG8" s="58"/>
+      <c r="AH8" s="71"/>
+      <c r="AI8" s="57"/>
+      <c r="AJ8" s="57"/>
+      <c r="AK8" s="57"/>
+      <c r="AL8" s="58"/>
       <c r="AM8" s="24"/>
       <c r="AN8" s="24"/>
       <c r="AO8" s="24"/>
@@ -1778,59 +1784,59 @@
       <c r="BK8" s="25"/>
     </row>
     <row r="9" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="107" t="s">
+      <c r="B9" s="95"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="78"/>
-      <c r="J9" s="98" t="s">
+      <c r="I9" s="79"/>
+      <c r="J9" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="84"/>
-      <c r="R9" s="84"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="107" t="s">
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="85"/>
+      <c r="Q9" s="85"/>
+      <c r="R9" s="85"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="U9" s="94"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="107" t="s">
+      <c r="U9" s="95"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="X9" s="98"/>
-      <c r="Y9" s="84"/>
-      <c r="Z9" s="84"/>
-      <c r="AA9" s="84"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="100" t="s">
+      <c r="X9" s="99"/>
+      <c r="Y9" s="85"/>
+      <c r="Z9" s="85"/>
+      <c r="AA9" s="85"/>
+      <c r="AB9" s="86"/>
+      <c r="AC9" s="101" t="s">
         <v>30</v>
       </c>
       <c r="AD9" s="64"/>
       <c r="AE9" s="64"/>
       <c r="AF9" s="64"/>
       <c r="AG9" s="65"/>
-      <c r="AH9" s="100" t="s">
+      <c r="AH9" s="101" t="s">
         <v>31</v>
       </c>
       <c r="AI9" s="64"/>
       <c r="AJ9" s="64"/>
       <c r="AK9" s="64"/>
       <c r="AL9" s="65"/>
-      <c r="AM9" s="73"/>
+      <c r="AM9" s="77"/>
       <c r="AN9" s="64"/>
       <c r="AO9" s="64"/>
       <c r="AP9" s="64"/>
@@ -1879,7 +1885,7 @@
       <c r="T10" s="66"/>
       <c r="U10" s="67"/>
       <c r="V10" s="68"/>
-      <c r="W10" s="58"/>
+      <c r="W10" s="55"/>
       <c r="X10" s="66"/>
       <c r="Y10" s="67"/>
       <c r="Z10" s="67"/>
@@ -1922,7 +1928,7 @@
       <c r="BK10" s="68"/>
     </row>
     <row r="11" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="113" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="64"/>
@@ -1990,9 +1996,9 @@
       <c r="BK11" s="65"/>
     </row>
     <row r="12" spans="1:63" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="81"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="66"/>
       <c r="E12" s="67"/>
       <c r="F12" s="67"/>
@@ -2050,87 +2056,87 @@
       <c r="BK12" s="68"/>
     </row>
     <row r="13" spans="1:63" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="106" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="70"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="77" t="s">
+      <c r="C13" s="104"/>
+      <c r="D13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="78"/>
-      <c r="F13" s="88" t="s">
+      <c r="E13" s="79"/>
+      <c r="F13" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="55"/>
+      <c r="G13" s="58"/>
       <c r="H13" s="10"/>
       <c r="I13" s="18"/>
-      <c r="J13" s="99" t="s">
+      <c r="J13" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="99" t="s">
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="78"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="95"/>
+      <c r="R13" s="95"/>
+      <c r="S13" s="79"/>
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
-      <c r="X13" s="99" t="s">
+      <c r="X13" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="Y13" s="94"/>
-      <c r="Z13" s="94"/>
-      <c r="AA13" s="94"/>
-      <c r="AB13" s="78"/>
+      <c r="Y13" s="95"/>
+      <c r="Z13" s="95"/>
+      <c r="AA13" s="95"/>
+      <c r="AB13" s="79"/>
       <c r="AC13" s="18"/>
       <c r="AD13" s="18"/>
       <c r="AE13" s="18"/>
       <c r="AF13" s="18"/>
       <c r="AG13" s="18"/>
-      <c r="AH13" s="123" t="s">
+      <c r="AH13" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="AI13" s="54"/>
-      <c r="AJ13" s="54"/>
-      <c r="AK13" s="54"/>
-      <c r="AL13" s="55"/>
-      <c r="AM13" s="76" t="s">
+      <c r="AI13" s="57"/>
+      <c r="AJ13" s="57"/>
+      <c r="AK13" s="57"/>
+      <c r="AL13" s="58"/>
+      <c r="AM13" s="74" t="s">
         <v>43</v>
       </c>
       <c r="AN13" s="67"/>
       <c r="AO13" s="67"/>
       <c r="AP13" s="67"/>
       <c r="AQ13" s="68"/>
-      <c r="AR13" s="76" t="s">
+      <c r="AR13" s="74" t="s">
         <v>44</v>
       </c>
       <c r="AS13" s="67"/>
       <c r="AT13" s="67"/>
       <c r="AU13" s="67"/>
       <c r="AV13" s="68"/>
-      <c r="AW13" s="76" t="s">
+      <c r="AW13" s="74" t="s">
         <v>45</v>
       </c>
       <c r="AX13" s="67"/>
       <c r="AY13" s="67"/>
       <c r="AZ13" s="67"/>
       <c r="BA13" s="68"/>
-      <c r="BB13" s="76" t="s">
+      <c r="BB13" s="74" t="s">
         <v>46</v>
       </c>
       <c r="BC13" s="67"/>
       <c r="BD13" s="67"/>
       <c r="BE13" s="67"/>
       <c r="BF13" s="68"/>
-      <c r="BG13" s="76" t="s">
+      <c r="BG13" s="74" t="s">
         <v>47</v>
       </c>
       <c r="BH13" s="67"/>
@@ -2139,131 +2145,131 @@
       <c r="BK13" s="68"/>
     </row>
     <row r="14" spans="1:63" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D14" s="115" t="s">
+      <c r="D14" s="117" t="s">
         <v>48</v>
       </c>
       <c r="E14" s="65"/>
-      <c r="F14" s="116" t="s">
+      <c r="F14" s="118" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="65"/>
-      <c r="H14" s="53" t="s">
+      <c r="H14" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="55"/>
-      <c r="J14" s="41" t="s">
+      <c r="I14" s="58"/>
+      <c r="J14" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="53" t="s">
+      <c r="K14" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="41" t="s">
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="119" t="s">
+      <c r="P14" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="90" t="s">
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="U14" s="54"/>
-      <c r="V14" s="91"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="92"/>
       <c r="W14" s="26" t="s">
         <v>48</v>
       </c>
       <c r="X14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Y14" s="71" t="s">
+      <c r="Y14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="Z14" s="54"/>
-      <c r="AA14" s="54"/>
-      <c r="AB14" s="55"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="57"/>
+      <c r="AB14" s="58"/>
       <c r="AC14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AD14" s="71" t="s">
+      <c r="AD14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AE14" s="54"/>
-      <c r="AF14" s="54"/>
-      <c r="AG14" s="55"/>
+      <c r="AE14" s="57"/>
+      <c r="AF14" s="57"/>
+      <c r="AG14" s="58"/>
       <c r="AH14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AI14" s="71" t="s">
+      <c r="AI14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AJ14" s="54"/>
-      <c r="AK14" s="54"/>
-      <c r="AL14" s="55"/>
+      <c r="AJ14" s="57"/>
+      <c r="AK14" s="57"/>
+      <c r="AL14" s="58"/>
       <c r="AM14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AN14" s="71" t="s">
+      <c r="AN14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AO14" s="54"/>
-      <c r="AP14" s="54"/>
-      <c r="AQ14" s="55"/>
+      <c r="AO14" s="57"/>
+      <c r="AP14" s="57"/>
+      <c r="AQ14" s="58"/>
       <c r="AR14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AS14" s="71" t="s">
+      <c r="AS14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AT14" s="54"/>
-      <c r="AU14" s="54"/>
-      <c r="AV14" s="55"/>
+      <c r="AT14" s="57"/>
+      <c r="AU14" s="57"/>
+      <c r="AV14" s="58"/>
       <c r="AW14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="AX14" s="71" t="s">
+      <c r="AX14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AY14" s="54"/>
-      <c r="AZ14" s="54"/>
-      <c r="BA14" s="55"/>
+      <c r="AY14" s="57"/>
+      <c r="AZ14" s="57"/>
+      <c r="BA14" s="58"/>
       <c r="BB14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="BC14" s="71" t="s">
+      <c r="BC14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="BD14" s="54"/>
-      <c r="BE14" s="54"/>
-      <c r="BF14" s="55"/>
+      <c r="BD14" s="57"/>
+      <c r="BE14" s="57"/>
+      <c r="BF14" s="58"/>
       <c r="BG14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="BH14" s="71" t="s">
+      <c r="BH14" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="BI14" s="54"/>
-      <c r="BJ14" s="54"/>
-      <c r="BK14" s="55"/>
+      <c r="BI14" s="57"/>
+      <c r="BJ14" s="57"/>
+      <c r="BK14" s="58"/>
     </row>
     <row r="15" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D15" s="74">
-        <v>1</v>
-      </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="74">
-        <v>1</v>
-      </c>
-      <c r="G15" s="75"/>
-      <c r="H15" s="92">
-        <v>1</v>
-      </c>
-      <c r="I15" s="75"/>
-      <c r="J15" s="87">
+      <c r="D15" s="75">
+        <v>1</v>
+      </c>
+      <c r="E15" s="76"/>
+      <c r="F15" s="75">
+        <v>1</v>
+      </c>
+      <c r="G15" s="76"/>
+      <c r="H15" s="93">
+        <v>1</v>
+      </c>
+      <c r="I15" s="76"/>
+      <c r="J15" s="88">
         <v>1</v>
       </c>
       <c r="K15" s="42">
@@ -2278,7 +2284,7 @@
       <c r="N15" s="43">
         <v>4</v>
       </c>
-      <c r="O15" s="87">
+      <c r="O15" s="88">
         <v>1</v>
       </c>
       <c r="P15" s="44">
@@ -2293,18 +2299,18 @@
       <c r="S15" s="45">
         <v>4</v>
       </c>
-      <c r="T15" s="92">
-        <v>1</v>
-      </c>
-      <c r="U15" s="120"/>
-      <c r="V15" s="75"/>
-      <c r="W15" s="38">
-        <v>1</v>
-      </c>
-      <c r="X15" s="96">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="2">
+      <c r="T15" s="93">
+        <v>1</v>
+      </c>
+      <c r="U15" s="122"/>
+      <c r="V15" s="76"/>
+      <c r="W15" s="39">
+        <v>1</v>
+      </c>
+      <c r="X15" s="97">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="42">
         <v>1</v>
       </c>
       <c r="Z15" s="1">
@@ -2313,10 +2319,10 @@
       <c r="AA15" s="1">
         <v>3</v>
       </c>
-      <c r="AB15" s="3">
-        <v>4</v>
-      </c>
-      <c r="AC15" s="56">
+      <c r="AB15" s="43">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="53">
         <v>1</v>
       </c>
       <c r="AD15" s="7">
@@ -2331,7 +2337,7 @@
       <c r="AG15" s="9">
         <v>4</v>
       </c>
-      <c r="AH15" s="56">
+      <c r="AH15" s="53">
         <v>1</v>
       </c>
       <c r="AI15" s="7">
@@ -2346,7 +2352,7 @@
       <c r="AL15" s="9">
         <v>4</v>
       </c>
-      <c r="AM15" s="56">
+      <c r="AM15" s="53">
         <v>1</v>
       </c>
       <c r="AN15" s="2">
@@ -2361,7 +2367,7 @@
       <c r="AQ15" s="3">
         <v>4</v>
       </c>
-      <c r="AR15" s="56">
+      <c r="AR15" s="53">
         <v>1</v>
       </c>
       <c r="AS15" s="2">
@@ -2376,7 +2382,7 @@
       <c r="AV15" s="3">
         <v>4</v>
       </c>
-      <c r="AW15" s="56">
+      <c r="AW15" s="53">
         <v>1</v>
       </c>
       <c r="AX15" s="2">
@@ -2391,7 +2397,7 @@
       <c r="BA15" s="3">
         <v>4</v>
       </c>
-      <c r="BB15" s="56">
+      <c r="BB15" s="53">
         <v>1</v>
       </c>
       <c r="BC15" s="2">
@@ -2406,7 +2412,7 @@
       <c r="BF15" s="3">
         <v>4</v>
       </c>
-      <c r="BG15" s="56">
+      <c r="BG15" s="53">
         <v>1</v>
       </c>
       <c r="BH15" s="2">
@@ -2435,7 +2441,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="62"/>
-      <c r="J16" s="57"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="42">
         <v>5</v>
       </c>
@@ -2448,7 +2454,7 @@
       <c r="N16" s="43">
         <v>8</v>
       </c>
-      <c r="O16" s="57"/>
+      <c r="O16" s="54"/>
       <c r="P16" s="42">
         <v>5</v>
       </c>
@@ -2464,13 +2470,13 @@
       <c r="T16" s="61">
         <v>2</v>
       </c>
-      <c r="U16" s="104"/>
+      <c r="U16" s="105"/>
       <c r="V16" s="62"/>
-      <c r="W16" s="39">
+      <c r="W16" s="40">
         <v>2</v>
       </c>
-      <c r="X16" s="78"/>
-      <c r="Y16" s="2">
+      <c r="X16" s="79"/>
+      <c r="Y16" s="42">
         <v>5</v>
       </c>
       <c r="Z16" s="1">
@@ -2479,10 +2485,10 @@
       <c r="AA16" s="1">
         <v>7</v>
       </c>
-      <c r="AB16" s="3">
+      <c r="AB16" s="43">
         <v>8</v>
       </c>
-      <c r="AC16" s="57"/>
+      <c r="AC16" s="54"/>
       <c r="AD16" s="2">
         <v>5</v>
       </c>
@@ -2495,7 +2501,7 @@
       <c r="AG16" s="3">
         <v>8</v>
       </c>
-      <c r="AH16" s="57"/>
+      <c r="AH16" s="54"/>
       <c r="AI16" s="2">
         <v>5</v>
       </c>
@@ -2508,7 +2514,7 @@
       <c r="AL16" s="3">
         <v>8</v>
       </c>
-      <c r="AM16" s="57"/>
+      <c r="AM16" s="54"/>
       <c r="AN16" s="2">
         <v>5</v>
       </c>
@@ -2521,7 +2527,7 @@
       <c r="AQ16" s="3">
         <v>8</v>
       </c>
-      <c r="AR16" s="57"/>
+      <c r="AR16" s="54"/>
       <c r="AS16" s="2">
         <v>5</v>
       </c>
@@ -2534,7 +2540,7 @@
       <c r="AV16" s="3">
         <v>8</v>
       </c>
-      <c r="AW16" s="57"/>
+      <c r="AW16" s="54"/>
       <c r="AX16" s="2">
         <v>5</v>
       </c>
@@ -2547,7 +2553,7 @@
       <c r="BA16" s="3">
         <v>8</v>
       </c>
-      <c r="BB16" s="57"/>
+      <c r="BB16" s="54"/>
       <c r="BC16" s="2">
         <v>5</v>
       </c>
@@ -2560,7 +2566,7 @@
       <c r="BF16" s="3">
         <v>8</v>
       </c>
-      <c r="BG16" s="57"/>
+      <c r="BG16" s="54"/>
       <c r="BH16" s="2">
         <v>5</v>
       </c>
@@ -2575,11 +2581,11 @@
       </c>
     </row>
     <row r="17" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="D17" s="95">
+      <c r="D17" s="96">
         <v>3</v>
       </c>
       <c r="E17" s="62"/>
-      <c r="F17" s="95">
+      <c r="F17" s="96">
         <v>3</v>
       </c>
       <c r="G17" s="62"/>
@@ -2587,7 +2593,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="62"/>
-      <c r="J17" s="57"/>
+      <c r="J17" s="54"/>
       <c r="K17" s="42">
         <v>9</v>
       </c>
@@ -2600,7 +2606,7 @@
       <c r="N17" s="43">
         <v>12</v>
       </c>
-      <c r="O17" s="57"/>
+      <c r="O17" s="54"/>
       <c r="P17" s="42">
         <v>9</v>
       </c>
@@ -2616,13 +2622,13 @@
       <c r="T17" s="61">
         <v>3</v>
       </c>
-      <c r="U17" s="104"/>
+      <c r="U17" s="105"/>
       <c r="V17" s="62"/>
-      <c r="W17" s="39">
-        <v>3</v>
-      </c>
-      <c r="X17" s="78"/>
-      <c r="Y17" s="2">
+      <c r="W17" s="40">
+        <v>3</v>
+      </c>
+      <c r="X17" s="79"/>
+      <c r="Y17" s="42">
         <v>9</v>
       </c>
       <c r="Z17" s="1">
@@ -2631,10 +2637,10 @@
       <c r="AA17" s="1">
         <v>11</v>
       </c>
-      <c r="AB17" s="3">
+      <c r="AB17" s="43">
         <v>12</v>
       </c>
-      <c r="AC17" s="57"/>
+      <c r="AC17" s="54"/>
       <c r="AD17" s="2">
         <v>9</v>
       </c>
@@ -2647,7 +2653,7 @@
       <c r="AG17" s="3">
         <v>12</v>
       </c>
-      <c r="AH17" s="57"/>
+      <c r="AH17" s="54"/>
       <c r="AI17" s="2">
         <v>9</v>
       </c>
@@ -2660,7 +2666,7 @@
       <c r="AL17" s="3">
         <v>12</v>
       </c>
-      <c r="AM17" s="57"/>
+      <c r="AM17" s="54"/>
       <c r="AN17" s="2">
         <v>9</v>
       </c>
@@ -2673,7 +2679,7 @@
       <c r="AQ17" s="3">
         <v>12</v>
       </c>
-      <c r="AR17" s="57"/>
+      <c r="AR17" s="54"/>
       <c r="AS17" s="2">
         <v>9</v>
       </c>
@@ -2686,7 +2692,7 @@
       <c r="AV17" s="3">
         <v>12</v>
       </c>
-      <c r="AW17" s="57"/>
+      <c r="AW17" s="54"/>
       <c r="AX17" s="2">
         <v>9</v>
       </c>
@@ -2699,7 +2705,7 @@
       <c r="BA17" s="3">
         <v>12</v>
       </c>
-      <c r="BB17" s="57"/>
+      <c r="BB17" s="54"/>
       <c r="BC17" s="2">
         <v>9</v>
       </c>
@@ -2712,7 +2718,7 @@
       <c r="BF17" s="3">
         <v>12</v>
       </c>
-      <c r="BG17" s="57"/>
+      <c r="BG17" s="54"/>
       <c r="BH17" s="2">
         <v>9</v>
       </c>
@@ -2727,11 +2733,11 @@
       </c>
     </row>
     <row r="18" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="D18" s="95">
+      <c r="D18" s="96">
         <v>4</v>
       </c>
       <c r="E18" s="62"/>
-      <c r="F18" s="95">
+      <c r="F18" s="96">
         <v>4</v>
       </c>
       <c r="G18" s="62"/>
@@ -2739,7 +2745,7 @@
         <v>4</v>
       </c>
       <c r="I18" s="62"/>
-      <c r="J18" s="57"/>
+      <c r="J18" s="54"/>
       <c r="K18" s="42">
         <v>13</v>
       </c>
@@ -2752,7 +2758,7 @@
       <c r="N18" s="43">
         <v>16</v>
       </c>
-      <c r="O18" s="57"/>
+      <c r="O18" s="54"/>
       <c r="P18" s="42">
         <v>13</v>
       </c>
@@ -2768,13 +2774,13 @@
       <c r="T18" s="61">
         <v>4</v>
       </c>
-      <c r="U18" s="104"/>
+      <c r="U18" s="105"/>
       <c r="V18" s="62"/>
-      <c r="W18" s="39">
-        <v>4</v>
-      </c>
-      <c r="X18" s="78"/>
-      <c r="Y18" s="2">
+      <c r="W18" s="40">
+        <v>4</v>
+      </c>
+      <c r="X18" s="79"/>
+      <c r="Y18" s="42">
         <v>13</v>
       </c>
       <c r="Z18" s="1">
@@ -2783,10 +2789,10 @@
       <c r="AA18" s="1">
         <v>15</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AB18" s="43">
         <v>16</v>
       </c>
-      <c r="AC18" s="57"/>
+      <c r="AC18" s="54"/>
       <c r="AD18" s="2">
         <v>13</v>
       </c>
@@ -2799,7 +2805,7 @@
       <c r="AG18" s="3">
         <v>16</v>
       </c>
-      <c r="AH18" s="57"/>
+      <c r="AH18" s="54"/>
       <c r="AI18" s="2">
         <v>13</v>
       </c>
@@ -2812,7 +2818,7 @@
       <c r="AL18" s="3">
         <v>16</v>
       </c>
-      <c r="AM18" s="57"/>
+      <c r="AM18" s="54"/>
       <c r="AN18" s="2">
         <v>13</v>
       </c>
@@ -2825,7 +2831,7 @@
       <c r="AQ18" s="3">
         <v>16</v>
       </c>
-      <c r="AR18" s="57"/>
+      <c r="AR18" s="54"/>
       <c r="AS18" s="2">
         <v>13</v>
       </c>
@@ -2838,7 +2844,7 @@
       <c r="AV18" s="3">
         <v>16</v>
       </c>
-      <c r="AW18" s="57"/>
+      <c r="AW18" s="54"/>
       <c r="AX18" s="2">
         <v>13</v>
       </c>
@@ -2851,7 +2857,7 @@
       <c r="BA18" s="3">
         <v>16</v>
       </c>
-      <c r="BB18" s="57"/>
+      <c r="BB18" s="54"/>
       <c r="BC18" s="2">
         <v>13</v>
       </c>
@@ -2864,7 +2870,7 @@
       <c r="BF18" s="3">
         <v>16</v>
       </c>
-      <c r="BG18" s="57"/>
+      <c r="BG18" s="54"/>
       <c r="BH18" s="2">
         <v>13</v>
       </c>
@@ -2879,7 +2885,7 @@
       </c>
     </row>
     <row r="19" spans="4:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D19" s="95">
+      <c r="D19" s="96">
         <v>5</v>
       </c>
       <c r="E19" s="62"/>
@@ -2891,7 +2897,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="62"/>
-      <c r="J19" s="58"/>
+      <c r="J19" s="55"/>
       <c r="K19" s="47">
         <v>17</v>
       </c>
@@ -2904,7 +2910,7 @@
       <c r="N19" s="48">
         <v>20</v>
       </c>
-      <c r="O19" s="58"/>
+      <c r="O19" s="55"/>
       <c r="P19" s="47">
         <v>17</v>
       </c>
@@ -2920,13 +2926,13 @@
       <c r="T19" s="61">
         <v>5</v>
       </c>
-      <c r="U19" s="104"/>
+      <c r="U19" s="105"/>
       <c r="V19" s="62"/>
-      <c r="W19" s="39">
+      <c r="W19" s="40">
         <v>5</v>
       </c>
       <c r="X19" s="68"/>
-      <c r="Y19" s="4">
+      <c r="Y19" s="47">
         <v>17</v>
       </c>
       <c r="Z19" s="5">
@@ -2935,10 +2941,10 @@
       <c r="AA19" s="5">
         <v>19</v>
       </c>
-      <c r="AB19" s="6">
+      <c r="AB19" s="48">
         <v>20</v>
       </c>
-      <c r="AC19" s="58"/>
+      <c r="AC19" s="55"/>
       <c r="AD19" s="4">
         <v>17</v>
       </c>
@@ -2951,7 +2957,7 @@
       <c r="AG19" s="6">
         <v>20</v>
       </c>
-      <c r="AH19" s="58"/>
+      <c r="AH19" s="55"/>
       <c r="AI19" s="4">
         <v>17</v>
       </c>
@@ -2964,7 +2970,7 @@
       <c r="AL19" s="6">
         <v>20</v>
       </c>
-      <c r="AM19" s="58"/>
+      <c r="AM19" s="55"/>
       <c r="AN19" s="4">
         <v>17</v>
       </c>
@@ -2977,7 +2983,7 @@
       <c r="AQ19" s="6">
         <v>20</v>
       </c>
-      <c r="AR19" s="58"/>
+      <c r="AR19" s="55"/>
       <c r="AS19" s="4">
         <v>17</v>
       </c>
@@ -2990,7 +2996,7 @@
       <c r="AV19" s="6">
         <v>20</v>
       </c>
-      <c r="AW19" s="58"/>
+      <c r="AW19" s="55"/>
       <c r="AX19" s="4">
         <v>17</v>
       </c>
@@ -3003,7 +3009,7 @@
       <c r="BA19" s="6">
         <v>20</v>
       </c>
-      <c r="BB19" s="58"/>
+      <c r="BB19" s="55"/>
       <c r="BC19" s="4">
         <v>17</v>
       </c>
@@ -3016,7 +3022,7 @@
       <c r="BF19" s="6">
         <v>20</v>
       </c>
-      <c r="BG19" s="58"/>
+      <c r="BG19" s="55"/>
       <c r="BH19" s="4">
         <v>17</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>6</v>
       </c>
       <c r="I20" s="52"/>
-      <c r="J20" s="87">
+      <c r="J20" s="88">
         <v>2</v>
       </c>
       <c r="K20" s="7">
@@ -3058,7 +3064,7 @@
       <c r="N20" s="9">
         <v>4</v>
       </c>
-      <c r="O20" s="87">
+      <c r="O20" s="88">
         <v>2</v>
       </c>
       <c r="P20" s="7">
@@ -3076,12 +3082,12 @@
       <c r="T20" s="51">
         <v>6</v>
       </c>
-      <c r="U20" s="89"/>
+      <c r="U20" s="90"/>
       <c r="V20" s="52"/>
-      <c r="W20" s="40">
-        <v>6</v>
-      </c>
-      <c r="X20" s="56">
+      <c r="W20" s="41">
+        <v>6</v>
+      </c>
+      <c r="X20" s="73">
         <v>2</v>
       </c>
       <c r="Y20" s="7">
@@ -3096,7 +3102,7 @@
       <c r="AB20" s="9">
         <v>4</v>
       </c>
-      <c r="AC20" s="56">
+      <c r="AC20" s="53">
         <v>2</v>
       </c>
       <c r="AD20" s="7">
@@ -3111,7 +3117,7 @@
       <c r="AG20" s="9">
         <v>4</v>
       </c>
-      <c r="AH20" s="56">
+      <c r="AH20" s="53">
         <v>2</v>
       </c>
       <c r="AI20" s="7">
@@ -3126,7 +3132,7 @@
       <c r="AL20" s="9">
         <v>4</v>
       </c>
-      <c r="AM20" s="56">
+      <c r="AM20" s="53">
         <v>2</v>
       </c>
       <c r="AN20" s="7">
@@ -3141,7 +3147,7 @@
       <c r="AQ20" s="9">
         <v>4</v>
       </c>
-      <c r="AR20" s="56">
+      <c r="AR20" s="53">
         <v>2</v>
       </c>
       <c r="AS20" s="7">
@@ -3156,7 +3162,7 @@
       <c r="AV20" s="9">
         <v>4</v>
       </c>
-      <c r="AW20" s="56">
+      <c r="AW20" s="53">
         <v>2</v>
       </c>
       <c r="AX20" s="7">
@@ -3171,7 +3177,7 @@
       <c r="BA20" s="9">
         <v>4</v>
       </c>
-      <c r="BB20" s="56">
+      <c r="BB20" s="53">
         <v>2</v>
       </c>
       <c r="BC20" s="7">
@@ -3186,7 +3192,7 @@
       <c r="BF20" s="9">
         <v>4</v>
       </c>
-      <c r="BG20" s="56">
+      <c r="BG20" s="53">
         <v>2</v>
       </c>
       <c r="BH20" s="7">
@@ -3203,7 +3209,7 @@
       </c>
     </row>
     <row r="21" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J21" s="57"/>
+      <c r="J21" s="54"/>
       <c r="K21" s="2">
         <v>5</v>
       </c>
@@ -3216,7 +3222,7 @@
       <c r="N21" s="3">
         <v>8</v>
       </c>
-      <c r="O21" s="57"/>
+      <c r="O21" s="54"/>
       <c r="P21" s="2">
         <v>5</v>
       </c>
@@ -3229,7 +3235,7 @@
       <c r="S21" s="3">
         <v>8</v>
       </c>
-      <c r="X21" s="57"/>
+      <c r="X21" s="54"/>
       <c r="Y21" s="2">
         <v>5</v>
       </c>
@@ -3242,7 +3248,7 @@
       <c r="AB21" s="3">
         <v>8</v>
       </c>
-      <c r="AC21" s="57"/>
+      <c r="AC21" s="54"/>
       <c r="AD21" s="2">
         <v>5</v>
       </c>
@@ -3255,7 +3261,7 @@
       <c r="AG21" s="3">
         <v>8</v>
       </c>
-      <c r="AH21" s="57"/>
+      <c r="AH21" s="54"/>
       <c r="AI21" s="2">
         <v>5</v>
       </c>
@@ -3268,7 +3274,7 @@
       <c r="AL21" s="3">
         <v>8</v>
       </c>
-      <c r="AM21" s="57"/>
+      <c r="AM21" s="54"/>
       <c r="AN21" s="2">
         <v>5</v>
       </c>
@@ -3281,7 +3287,7 @@
       <c r="AQ21" s="3">
         <v>8</v>
       </c>
-      <c r="AR21" s="57"/>
+      <c r="AR21" s="54"/>
       <c r="AS21" s="2">
         <v>5</v>
       </c>
@@ -3294,7 +3300,7 @@
       <c r="AV21" s="3">
         <v>8</v>
       </c>
-      <c r="AW21" s="57"/>
+      <c r="AW21" s="54"/>
       <c r="AX21" s="2">
         <v>5</v>
       </c>
@@ -3307,7 +3313,7 @@
       <c r="BA21" s="3">
         <v>8</v>
       </c>
-      <c r="BB21" s="57"/>
+      <c r="BB21" s="54"/>
       <c r="BC21" s="2">
         <v>5</v>
       </c>
@@ -3320,7 +3326,7 @@
       <c r="BF21" s="3">
         <v>8</v>
       </c>
-      <c r="BG21" s="57"/>
+      <c r="BG21" s="54"/>
       <c r="BH21" s="2">
         <v>5</v>
       </c>
@@ -3335,7 +3341,7 @@
       </c>
     </row>
     <row r="22" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J22" s="57"/>
+      <c r="J22" s="54"/>
       <c r="K22" s="2">
         <v>9</v>
       </c>
@@ -3348,7 +3354,7 @@
       <c r="N22" s="3">
         <v>12</v>
       </c>
-      <c r="O22" s="57"/>
+      <c r="O22" s="54"/>
       <c r="P22" s="2">
         <v>9</v>
       </c>
@@ -3361,7 +3367,7 @@
       <c r="S22" s="3">
         <v>12</v>
       </c>
-      <c r="X22" s="57"/>
+      <c r="X22" s="54"/>
       <c r="Y22" s="2">
         <v>9</v>
       </c>
@@ -3374,7 +3380,7 @@
       <c r="AB22" s="3">
         <v>12</v>
       </c>
-      <c r="AC22" s="57"/>
+      <c r="AC22" s="54"/>
       <c r="AD22" s="2">
         <v>9</v>
       </c>
@@ -3387,7 +3393,7 @@
       <c r="AG22" s="3">
         <v>12</v>
       </c>
-      <c r="AH22" s="57"/>
+      <c r="AH22" s="54"/>
       <c r="AI22" s="2">
         <v>9</v>
       </c>
@@ -3400,7 +3406,7 @@
       <c r="AL22" s="3">
         <v>12</v>
       </c>
-      <c r="AM22" s="57"/>
+      <c r="AM22" s="54"/>
       <c r="AN22" s="2">
         <v>9</v>
       </c>
@@ -3413,7 +3419,7 @@
       <c r="AQ22" s="3">
         <v>12</v>
       </c>
-      <c r="AR22" s="57"/>
+      <c r="AR22" s="54"/>
       <c r="AS22" s="2">
         <v>9</v>
       </c>
@@ -3426,7 +3432,7 @@
       <c r="AV22" s="3">
         <v>12</v>
       </c>
-      <c r="AW22" s="57"/>
+      <c r="AW22" s="54"/>
       <c r="AX22" s="2">
         <v>9</v>
       </c>
@@ -3439,7 +3445,7 @@
       <c r="BA22" s="3">
         <v>12</v>
       </c>
-      <c r="BB22" s="57"/>
+      <c r="BB22" s="54"/>
       <c r="BC22" s="2">
         <v>9</v>
       </c>
@@ -3452,7 +3458,7 @@
       <c r="BF22" s="3">
         <v>12</v>
       </c>
-      <c r="BG22" s="57"/>
+      <c r="BG22" s="54"/>
       <c r="BH22" s="2">
         <v>9</v>
       </c>
@@ -3467,7 +3473,7 @@
       </c>
     </row>
     <row r="23" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J23" s="57"/>
+      <c r="J23" s="54"/>
       <c r="K23" s="2">
         <v>13</v>
       </c>
@@ -3480,7 +3486,7 @@
       <c r="N23" s="3">
         <v>16</v>
       </c>
-      <c r="O23" s="57"/>
+      <c r="O23" s="54"/>
       <c r="P23" s="2">
         <v>13</v>
       </c>
@@ -3493,7 +3499,7 @@
       <c r="S23" s="3">
         <v>16</v>
       </c>
-      <c r="X23" s="57"/>
+      <c r="X23" s="54"/>
       <c r="Y23" s="2">
         <v>13</v>
       </c>
@@ -3506,7 +3512,7 @@
       <c r="AB23" s="3">
         <v>16</v>
       </c>
-      <c r="AC23" s="57"/>
+      <c r="AC23" s="54"/>
       <c r="AD23" s="2">
         <v>13</v>
       </c>
@@ -3519,7 +3525,7 @@
       <c r="AG23" s="3">
         <v>16</v>
       </c>
-      <c r="AH23" s="57"/>
+      <c r="AH23" s="54"/>
       <c r="AI23" s="2">
         <v>13</v>
       </c>
@@ -3532,7 +3538,7 @@
       <c r="AL23" s="3">
         <v>16</v>
       </c>
-      <c r="AM23" s="57"/>
+      <c r="AM23" s="54"/>
       <c r="AN23" s="2">
         <v>13</v>
       </c>
@@ -3545,7 +3551,7 @@
       <c r="AQ23" s="3">
         <v>16</v>
       </c>
-      <c r="AR23" s="57"/>
+      <c r="AR23" s="54"/>
       <c r="AS23" s="2">
         <v>13</v>
       </c>
@@ -3558,7 +3564,7 @@
       <c r="AV23" s="3">
         <v>16</v>
       </c>
-      <c r="AW23" s="57"/>
+      <c r="AW23" s="54"/>
       <c r="AX23" s="2">
         <v>13</v>
       </c>
@@ -3571,7 +3577,7 @@
       <c r="BA23" s="3">
         <v>16</v>
       </c>
-      <c r="BB23" s="57"/>
+      <c r="BB23" s="54"/>
       <c r="BC23" s="2">
         <v>13</v>
       </c>
@@ -3584,7 +3590,7 @@
       <c r="BF23" s="3">
         <v>16</v>
       </c>
-      <c r="BG23" s="57"/>
+      <c r="BG23" s="54"/>
       <c r="BH23" s="2">
         <v>13</v>
       </c>
@@ -3599,7 +3605,7 @@
       </c>
     </row>
     <row r="24" spans="4:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J24" s="58"/>
+      <c r="J24" s="55"/>
       <c r="K24" s="4">
         <v>17</v>
       </c>
@@ -3612,7 +3618,7 @@
       <c r="N24" s="6">
         <v>20</v>
       </c>
-      <c r="O24" s="58"/>
+      <c r="O24" s="55"/>
       <c r="P24" s="4">
         <v>17</v>
       </c>
@@ -3625,7 +3631,7 @@
       <c r="S24" s="6">
         <v>20</v>
       </c>
-      <c r="X24" s="58"/>
+      <c r="X24" s="55"/>
       <c r="Y24" s="4">
         <v>17</v>
       </c>
@@ -3638,7 +3644,7 @@
       <c r="AB24" s="6">
         <v>20</v>
       </c>
-      <c r="AC24" s="58"/>
+      <c r="AC24" s="55"/>
       <c r="AD24" s="4">
         <v>17</v>
       </c>
@@ -3651,7 +3657,7 @@
       <c r="AG24" s="6">
         <v>20</v>
       </c>
-      <c r="AH24" s="58"/>
+      <c r="AH24" s="55"/>
       <c r="AI24" s="4">
         <v>17</v>
       </c>
@@ -3664,7 +3670,7 @@
       <c r="AL24" s="6">
         <v>20</v>
       </c>
-      <c r="AM24" s="58"/>
+      <c r="AM24" s="55"/>
       <c r="AN24" s="4">
         <v>17</v>
       </c>
@@ -3677,7 +3683,7 @@
       <c r="AQ24" s="6">
         <v>20</v>
       </c>
-      <c r="AR24" s="58"/>
+      <c r="AR24" s="55"/>
       <c r="AS24" s="4">
         <v>17</v>
       </c>
@@ -3690,7 +3696,7 @@
       <c r="AV24" s="6">
         <v>20</v>
       </c>
-      <c r="AW24" s="58"/>
+      <c r="AW24" s="55"/>
       <c r="AX24" s="4">
         <v>17</v>
       </c>
@@ -3703,7 +3709,7 @@
       <c r="BA24" s="6">
         <v>20</v>
       </c>
-      <c r="BB24" s="58"/>
+      <c r="BB24" s="55"/>
       <c r="BC24" s="4">
         <v>17</v>
       </c>
@@ -3716,7 +3722,7 @@
       <c r="BF24" s="6">
         <v>20</v>
       </c>
-      <c r="BG24" s="58"/>
+      <c r="BG24" s="55"/>
       <c r="BH24" s="4">
         <v>17</v>
       </c>
@@ -3731,7 +3737,7 @@
       </c>
     </row>
     <row r="25" spans="4:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J25" s="87">
+      <c r="J25" s="88">
         <v>3</v>
       </c>
       <c r="K25" s="44">
@@ -3746,7 +3752,7 @@
       <c r="N25" s="50">
         <v>4</v>
       </c>
-      <c r="O25" s="87">
+      <c r="O25" s="88">
         <v>3</v>
       </c>
       <c r="P25" s="44">
@@ -3761,10 +3767,10 @@
       <c r="S25" s="50">
         <v>4</v>
       </c>
-      <c r="X25" s="56">
-        <v>3</v>
-      </c>
-      <c r="Y25" s="7">
+      <c r="X25" s="73">
+        <v>3</v>
+      </c>
+      <c r="Y25" s="44">
         <v>1</v>
       </c>
       <c r="Z25" s="8">
@@ -3773,10 +3779,10 @@
       <c r="AA25" s="8">
         <v>3</v>
       </c>
-      <c r="AB25" s="9">
-        <v>4</v>
-      </c>
-      <c r="AC25" s="56">
+      <c r="AB25" s="50">
+        <v>4</v>
+      </c>
+      <c r="AC25" s="53">
         <v>3</v>
       </c>
       <c r="AD25" s="7">
@@ -3791,7 +3797,7 @@
       <c r="AG25" s="9">
         <v>4</v>
       </c>
-      <c r="AH25" s="56">
+      <c r="AH25" s="53">
         <v>3</v>
       </c>
       <c r="AI25" s="7">
@@ -3806,7 +3812,7 @@
       <c r="AL25" s="9">
         <v>4</v>
       </c>
-      <c r="AM25" s="56">
+      <c r="AM25" s="53">
         <v>3</v>
       </c>
       <c r="AN25" s="7">
@@ -3821,7 +3827,7 @@
       <c r="AQ25" s="9">
         <v>4</v>
       </c>
-      <c r="AR25" s="56">
+      <c r="AR25" s="53">
         <v>3</v>
       </c>
       <c r="AS25" s="7">
@@ -3836,7 +3842,7 @@
       <c r="AV25" s="9">
         <v>4</v>
       </c>
-      <c r="AW25" s="56">
+      <c r="AW25" s="53">
         <v>3</v>
       </c>
       <c r="AX25" s="7">
@@ -3851,7 +3857,7 @@
       <c r="BA25" s="9">
         <v>4</v>
       </c>
-      <c r="BB25" s="56">
+      <c r="BB25" s="53">
         <v>3</v>
       </c>
       <c r="BC25" s="7">
@@ -3866,7 +3872,7 @@
       <c r="BF25" s="9">
         <v>4</v>
       </c>
-      <c r="BG25" s="56">
+      <c r="BG25" s="53">
         <v>3</v>
       </c>
       <c r="BH25" s="7">
@@ -3883,7 +3889,7 @@
       </c>
     </row>
     <row r="26" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J26" s="57"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="42">
         <v>5</v>
       </c>
@@ -3896,7 +3902,7 @@
       <c r="N26" s="43">
         <v>8</v>
       </c>
-      <c r="O26" s="57"/>
+      <c r="O26" s="54"/>
       <c r="P26" s="42">
         <v>5</v>
       </c>
@@ -3909,8 +3915,8 @@
       <c r="S26" s="43">
         <v>8</v>
       </c>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="2">
+      <c r="X26" s="54"/>
+      <c r="Y26" s="42">
         <v>5</v>
       </c>
       <c r="Z26" s="1">
@@ -3919,10 +3925,10 @@
       <c r="AA26" s="1">
         <v>7</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AB26" s="43">
         <v>8</v>
       </c>
-      <c r="AC26" s="57"/>
+      <c r="AC26" s="54"/>
       <c r="AD26" s="2">
         <v>5</v>
       </c>
@@ -3935,7 +3941,7 @@
       <c r="AG26" s="3">
         <v>8</v>
       </c>
-      <c r="AH26" s="57"/>
+      <c r="AH26" s="54"/>
       <c r="AI26" s="2">
         <v>5</v>
       </c>
@@ -3948,7 +3954,7 @@
       <c r="AL26" s="3">
         <v>8</v>
       </c>
-      <c r="AM26" s="57"/>
+      <c r="AM26" s="54"/>
       <c r="AN26" s="2">
         <v>5</v>
       </c>
@@ -3961,7 +3967,7 @@
       <c r="AQ26" s="3">
         <v>8</v>
       </c>
-      <c r="AR26" s="57"/>
+      <c r="AR26" s="54"/>
       <c r="AS26" s="2">
         <v>5</v>
       </c>
@@ -3974,7 +3980,7 @@
       <c r="AV26" s="3">
         <v>8</v>
       </c>
-      <c r="AW26" s="57"/>
+      <c r="AW26" s="54"/>
       <c r="AX26" s="2">
         <v>5</v>
       </c>
@@ -3987,7 +3993,7 @@
       <c r="BA26" s="3">
         <v>8</v>
       </c>
-      <c r="BB26" s="57"/>
+      <c r="BB26" s="54"/>
       <c r="BC26" s="2">
         <v>5</v>
       </c>
@@ -4000,7 +4006,7 @@
       <c r="BF26" s="3">
         <v>8</v>
       </c>
-      <c r="BG26" s="57"/>
+      <c r="BG26" s="54"/>
       <c r="BH26" s="2">
         <v>5</v>
       </c>
@@ -4015,7 +4021,7 @@
       </c>
     </row>
     <row r="27" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J27" s="57"/>
+      <c r="J27" s="54"/>
       <c r="K27" s="42">
         <v>9</v>
       </c>
@@ -4028,7 +4034,7 @@
       <c r="N27" s="43">
         <v>12</v>
       </c>
-      <c r="O27" s="57"/>
+      <c r="O27" s="54"/>
       <c r="P27" s="42">
         <v>9</v>
       </c>
@@ -4041,8 +4047,8 @@
       <c r="S27" s="43">
         <v>12</v>
       </c>
-      <c r="X27" s="57"/>
-      <c r="Y27" s="2">
+      <c r="X27" s="54"/>
+      <c r="Y27" s="42">
         <v>9</v>
       </c>
       <c r="Z27" s="1">
@@ -4051,10 +4057,10 @@
       <c r="AA27" s="1">
         <v>11</v>
       </c>
-      <c r="AB27" s="3">
+      <c r="AB27" s="43">
         <v>12</v>
       </c>
-      <c r="AC27" s="57"/>
+      <c r="AC27" s="54"/>
       <c r="AD27" s="2">
         <v>9</v>
       </c>
@@ -4067,7 +4073,7 @@
       <c r="AG27" s="3">
         <v>12</v>
       </c>
-      <c r="AH27" s="57"/>
+      <c r="AH27" s="54"/>
       <c r="AI27" s="2">
         <v>9</v>
       </c>
@@ -4080,7 +4086,7 @@
       <c r="AL27" s="3">
         <v>12</v>
       </c>
-      <c r="AM27" s="57"/>
+      <c r="AM27" s="54"/>
       <c r="AN27" s="2">
         <v>9</v>
       </c>
@@ -4093,7 +4099,7 @@
       <c r="AQ27" s="3">
         <v>12</v>
       </c>
-      <c r="AR27" s="57"/>
+      <c r="AR27" s="54"/>
       <c r="AS27" s="2">
         <v>9</v>
       </c>
@@ -4106,7 +4112,7 @@
       <c r="AV27" s="3">
         <v>12</v>
       </c>
-      <c r="AW27" s="57"/>
+      <c r="AW27" s="54"/>
       <c r="AX27" s="2">
         <v>9</v>
       </c>
@@ -4119,7 +4125,7 @@
       <c r="BA27" s="3">
         <v>12</v>
       </c>
-      <c r="BB27" s="57"/>
+      <c r="BB27" s="54"/>
       <c r="BC27" s="2">
         <v>9</v>
       </c>
@@ -4132,7 +4138,7 @@
       <c r="BF27" s="3">
         <v>12</v>
       </c>
-      <c r="BG27" s="57"/>
+      <c r="BG27" s="54"/>
       <c r="BH27" s="2">
         <v>9</v>
       </c>
@@ -4147,7 +4153,7 @@
       </c>
     </row>
     <row r="28" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J28" s="57"/>
+      <c r="J28" s="54"/>
       <c r="K28" s="42">
         <v>13</v>
       </c>
@@ -4160,7 +4166,7 @@
       <c r="N28" s="43">
         <v>16</v>
       </c>
-      <c r="O28" s="57"/>
+      <c r="O28" s="54"/>
       <c r="P28" s="42">
         <v>13</v>
       </c>
@@ -4173,8 +4179,8 @@
       <c r="S28" s="43">
         <v>16</v>
       </c>
-      <c r="X28" s="57"/>
-      <c r="Y28" s="2">
+      <c r="X28" s="54"/>
+      <c r="Y28" s="42">
         <v>13</v>
       </c>
       <c r="Z28" s="1">
@@ -4183,10 +4189,10 @@
       <c r="AA28" s="1">
         <v>15</v>
       </c>
-      <c r="AB28" s="3">
+      <c r="AB28" s="43">
         <v>16</v>
       </c>
-      <c r="AC28" s="57"/>
+      <c r="AC28" s="54"/>
       <c r="AD28" s="2">
         <v>13</v>
       </c>
@@ -4199,7 +4205,7 @@
       <c r="AG28" s="3">
         <v>16</v>
       </c>
-      <c r="AH28" s="57"/>
+      <c r="AH28" s="54"/>
       <c r="AI28" s="2">
         <v>13</v>
       </c>
@@ -4212,7 +4218,7 @@
       <c r="AL28" s="3">
         <v>16</v>
       </c>
-      <c r="AM28" s="57"/>
+      <c r="AM28" s="54"/>
       <c r="AN28" s="2">
         <v>13</v>
       </c>
@@ -4225,7 +4231,7 @@
       <c r="AQ28" s="3">
         <v>16</v>
       </c>
-      <c r="AR28" s="57"/>
+      <c r="AR28" s="54"/>
       <c r="AS28" s="2">
         <v>13</v>
       </c>
@@ -4238,7 +4244,7 @@
       <c r="AV28" s="3">
         <v>16</v>
       </c>
-      <c r="AW28" s="57"/>
+      <c r="AW28" s="54"/>
       <c r="AX28" s="2">
         <v>13</v>
       </c>
@@ -4251,7 +4257,7 @@
       <c r="BA28" s="3">
         <v>16</v>
       </c>
-      <c r="BB28" s="57"/>
+      <c r="BB28" s="54"/>
       <c r="BC28" s="2">
         <v>13</v>
       </c>
@@ -4264,7 +4270,7 @@
       <c r="BF28" s="3">
         <v>16</v>
       </c>
-      <c r="BG28" s="57"/>
+      <c r="BG28" s="54"/>
       <c r="BH28" s="2">
         <v>13</v>
       </c>
@@ -4279,7 +4285,7 @@
       </c>
     </row>
     <row r="29" spans="4:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J29" s="58"/>
+      <c r="J29" s="55"/>
       <c r="K29" s="47">
         <v>17</v>
       </c>
@@ -4292,7 +4298,7 @@
       <c r="N29" s="48">
         <v>20</v>
       </c>
-      <c r="O29" s="58"/>
+      <c r="O29" s="55"/>
       <c r="P29" s="47">
         <v>17</v>
       </c>
@@ -4305,8 +4311,8 @@
       <c r="S29" s="48">
         <v>20</v>
       </c>
-      <c r="X29" s="58"/>
-      <c r="Y29" s="4">
+      <c r="X29" s="55"/>
+      <c r="Y29" s="47">
         <v>17</v>
       </c>
       <c r="Z29" s="5">
@@ -4315,10 +4321,10 @@
       <c r="AA29" s="5">
         <v>19</v>
       </c>
-      <c r="AB29" s="6">
+      <c r="AB29" s="48">
         <v>20</v>
       </c>
-      <c r="AC29" s="58"/>
+      <c r="AC29" s="55"/>
       <c r="AD29" s="4">
         <v>17</v>
       </c>
@@ -4331,7 +4337,7 @@
       <c r="AG29" s="6">
         <v>20</v>
       </c>
-      <c r="AH29" s="58"/>
+      <c r="AH29" s="55"/>
       <c r="AI29" s="4">
         <v>17</v>
       </c>
@@ -4344,7 +4350,7 @@
       <c r="AL29" s="6">
         <v>20</v>
       </c>
-      <c r="AM29" s="58"/>
+      <c r="AM29" s="55"/>
       <c r="AN29" s="4">
         <v>17</v>
       </c>
@@ -4357,7 +4363,7 @@
       <c r="AQ29" s="6">
         <v>20</v>
       </c>
-      <c r="AR29" s="58"/>
+      <c r="AR29" s="55"/>
       <c r="AS29" s="4">
         <v>17</v>
       </c>
@@ -4370,7 +4376,7 @@
       <c r="AV29" s="6">
         <v>20</v>
       </c>
-      <c r="AW29" s="58"/>
+      <c r="AW29" s="55"/>
       <c r="AX29" s="4">
         <v>17</v>
       </c>
@@ -4383,7 +4389,7 @@
       <c r="BA29" s="6">
         <v>20</v>
       </c>
-      <c r="BB29" s="58"/>
+      <c r="BB29" s="55"/>
       <c r="BC29" s="4">
         <v>17</v>
       </c>
@@ -4396,7 +4402,7 @@
       <c r="BF29" s="6">
         <v>20</v>
       </c>
-      <c r="BG29" s="58"/>
+      <c r="BG29" s="55"/>
       <c r="BH29" s="4">
         <v>17</v>
       </c>
@@ -4411,7 +4417,7 @@
       </c>
     </row>
     <row r="30" spans="4:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J30" s="87">
+      <c r="J30" s="88">
         <v>4</v>
       </c>
       <c r="K30" s="44">
@@ -4426,7 +4432,7 @@
       <c r="N30" s="50">
         <v>4</v>
       </c>
-      <c r="O30" s="87">
+      <c r="O30" s="88">
         <v>4</v>
       </c>
       <c r="P30" s="44">
@@ -4441,10 +4447,10 @@
       <c r="S30" s="50">
         <v>4</v>
       </c>
-      <c r="X30" s="56">
-        <v>4</v>
-      </c>
-      <c r="Y30" s="7">
+      <c r="X30" s="73">
+        <v>4</v>
+      </c>
+      <c r="Y30" s="44">
         <v>1</v>
       </c>
       <c r="Z30" s="8">
@@ -4453,10 +4459,10 @@
       <c r="AA30" s="8">
         <v>3</v>
       </c>
-      <c r="AB30" s="9">
-        <v>4</v>
-      </c>
-      <c r="AC30" s="56">
+      <c r="AB30" s="50">
+        <v>4</v>
+      </c>
+      <c r="AC30" s="53">
         <v>4</v>
       </c>
       <c r="AD30" s="7">
@@ -4471,7 +4477,7 @@
       <c r="AG30" s="9">
         <v>4</v>
       </c>
-      <c r="AH30" s="56">
+      <c r="AH30" s="53">
         <v>4</v>
       </c>
       <c r="AI30" s="7">
@@ -4486,7 +4492,7 @@
       <c r="AL30" s="9">
         <v>4</v>
       </c>
-      <c r="AM30" s="56">
+      <c r="AM30" s="53">
         <v>4</v>
       </c>
       <c r="AN30" s="7">
@@ -4501,7 +4507,7 @@
       <c r="AQ30" s="9">
         <v>4</v>
       </c>
-      <c r="AR30" s="56">
+      <c r="AR30" s="53">
         <v>4</v>
       </c>
       <c r="AS30" s="7">
@@ -4516,7 +4522,7 @@
       <c r="AV30" s="9">
         <v>4</v>
       </c>
-      <c r="AW30" s="56">
+      <c r="AW30" s="53">
         <v>4</v>
       </c>
       <c r="AX30" s="7">
@@ -4531,7 +4537,7 @@
       <c r="BA30" s="9">
         <v>4</v>
       </c>
-      <c r="BB30" s="56">
+      <c r="BB30" s="53">
         <v>4</v>
       </c>
       <c r="BC30" s="7">
@@ -4546,7 +4552,7 @@
       <c r="BF30" s="9">
         <v>4</v>
       </c>
-      <c r="BG30" s="56">
+      <c r="BG30" s="53">
         <v>4</v>
       </c>
       <c r="BH30" s="7">
@@ -4563,7 +4569,7 @@
       </c>
     </row>
     <row r="31" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J31" s="57"/>
+      <c r="J31" s="54"/>
       <c r="K31" s="42">
         <v>5</v>
       </c>
@@ -4576,7 +4582,7 @@
       <c r="N31" s="43">
         <v>8</v>
       </c>
-      <c r="O31" s="57"/>
+      <c r="O31" s="54"/>
       <c r="P31" s="42">
         <v>5</v>
       </c>
@@ -4589,8 +4595,8 @@
       <c r="S31" s="43">
         <v>8</v>
       </c>
-      <c r="X31" s="57"/>
-      <c r="Y31" s="2">
+      <c r="X31" s="54"/>
+      <c r="Y31" s="42">
         <v>5</v>
       </c>
       <c r="Z31" s="1">
@@ -4599,10 +4605,10 @@
       <c r="AA31" s="1">
         <v>7</v>
       </c>
-      <c r="AB31" s="3">
+      <c r="AB31" s="43">
         <v>8</v>
       </c>
-      <c r="AC31" s="57"/>
+      <c r="AC31" s="54"/>
       <c r="AD31" s="2">
         <v>5</v>
       </c>
@@ -4615,7 +4621,7 @@
       <c r="AG31" s="3">
         <v>8</v>
       </c>
-      <c r="AH31" s="57"/>
+      <c r="AH31" s="54"/>
       <c r="AI31" s="2">
         <v>5</v>
       </c>
@@ -4628,7 +4634,7 @@
       <c r="AL31" s="3">
         <v>8</v>
       </c>
-      <c r="AM31" s="57"/>
+      <c r="AM31" s="54"/>
       <c r="AN31" s="2">
         <v>5</v>
       </c>
@@ -4641,7 +4647,7 @@
       <c r="AQ31" s="3">
         <v>8</v>
       </c>
-      <c r="AR31" s="57"/>
+      <c r="AR31" s="54"/>
       <c r="AS31" s="2">
         <v>5</v>
       </c>
@@ -4654,7 +4660,7 @@
       <c r="AV31" s="3">
         <v>8</v>
       </c>
-      <c r="AW31" s="57"/>
+      <c r="AW31" s="54"/>
       <c r="AX31" s="2">
         <v>5</v>
       </c>
@@ -4667,7 +4673,7 @@
       <c r="BA31" s="3">
         <v>8</v>
       </c>
-      <c r="BB31" s="57"/>
+      <c r="BB31" s="54"/>
       <c r="BC31" s="2">
         <v>5</v>
       </c>
@@ -4680,7 +4686,7 @@
       <c r="BF31" s="3">
         <v>8</v>
       </c>
-      <c r="BG31" s="57"/>
+      <c r="BG31" s="54"/>
       <c r="BH31" s="2">
         <v>5</v>
       </c>
@@ -4695,7 +4701,7 @@
       </c>
     </row>
     <row r="32" spans="4:63" x14ac:dyDescent="0.35">
-      <c r="J32" s="57"/>
+      <c r="J32" s="54"/>
       <c r="K32" s="42">
         <v>9</v>
       </c>
@@ -4708,7 +4714,7 @@
       <c r="N32" s="43">
         <v>12</v>
       </c>
-      <c r="O32" s="57"/>
+      <c r="O32" s="54"/>
       <c r="P32" s="42">
         <v>9</v>
       </c>
@@ -4721,8 +4727,8 @@
       <c r="S32" s="43">
         <v>12</v>
       </c>
-      <c r="X32" s="57"/>
-      <c r="Y32" s="2">
+      <c r="X32" s="54"/>
+      <c r="Y32" s="42">
         <v>9</v>
       </c>
       <c r="Z32" s="1">
@@ -4731,10 +4737,10 @@
       <c r="AA32" s="1">
         <v>11</v>
       </c>
-      <c r="AB32" s="3">
+      <c r="AB32" s="43">
         <v>12</v>
       </c>
-      <c r="AC32" s="57"/>
+      <c r="AC32" s="54"/>
       <c r="AD32" s="2">
         <v>9</v>
       </c>
@@ -4747,7 +4753,7 @@
       <c r="AG32" s="3">
         <v>12</v>
       </c>
-      <c r="AH32" s="57"/>
+      <c r="AH32" s="54"/>
       <c r="AI32" s="2">
         <v>9</v>
       </c>
@@ -4760,7 +4766,7 @@
       <c r="AL32" s="3">
         <v>12</v>
       </c>
-      <c r="AM32" s="57"/>
+      <c r="AM32" s="54"/>
       <c r="AN32" s="2">
         <v>9</v>
       </c>
@@ -4773,7 +4779,7 @@
       <c r="AQ32" s="3">
         <v>12</v>
       </c>
-      <c r="AR32" s="57"/>
+      <c r="AR32" s="54"/>
       <c r="AS32" s="2">
         <v>9</v>
       </c>
@@ -4786,7 +4792,7 @@
       <c r="AV32" s="3">
         <v>12</v>
       </c>
-      <c r="AW32" s="57"/>
+      <c r="AW32" s="54"/>
       <c r="AX32" s="2">
         <v>9</v>
       </c>
@@ -4799,7 +4805,7 @@
       <c r="BA32" s="3">
         <v>12</v>
       </c>
-      <c r="BB32" s="57"/>
+      <c r="BB32" s="54"/>
       <c r="BC32" s="2">
         <v>9</v>
       </c>
@@ -4812,7 +4818,7 @@
       <c r="BF32" s="3">
         <v>12</v>
       </c>
-      <c r="BG32" s="57"/>
+      <c r="BG32" s="54"/>
       <c r="BH32" s="2">
         <v>9</v>
       </c>
@@ -4827,7 +4833,7 @@
       </c>
     </row>
     <row r="33" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J33" s="57"/>
+      <c r="J33" s="54"/>
       <c r="K33" s="42">
         <v>13</v>
       </c>
@@ -4840,7 +4846,7 @@
       <c r="N33" s="43">
         <v>16</v>
       </c>
-      <c r="O33" s="57"/>
+      <c r="O33" s="54"/>
       <c r="P33" s="42">
         <v>13</v>
       </c>
@@ -4853,8 +4859,8 @@
       <c r="S33" s="43">
         <v>16</v>
       </c>
-      <c r="X33" s="57"/>
-      <c r="Y33" s="2">
+      <c r="X33" s="54"/>
+      <c r="Y33" s="42">
         <v>13</v>
       </c>
       <c r="Z33" s="1">
@@ -4863,10 +4869,10 @@
       <c r="AA33" s="1">
         <v>15</v>
       </c>
-      <c r="AB33" s="3">
+      <c r="AB33" s="43">
         <v>16</v>
       </c>
-      <c r="AC33" s="57"/>
+      <c r="AC33" s="54"/>
       <c r="AD33" s="2">
         <v>13</v>
       </c>
@@ -4879,7 +4885,7 @@
       <c r="AG33" s="3">
         <v>16</v>
       </c>
-      <c r="AH33" s="57"/>
+      <c r="AH33" s="54"/>
       <c r="AI33" s="2">
         <v>13</v>
       </c>
@@ -4892,7 +4898,7 @@
       <c r="AL33" s="3">
         <v>16</v>
       </c>
-      <c r="AM33" s="57"/>
+      <c r="AM33" s="54"/>
       <c r="AN33" s="2">
         <v>13</v>
       </c>
@@ -4905,7 +4911,7 @@
       <c r="AQ33" s="3">
         <v>16</v>
       </c>
-      <c r="AR33" s="57"/>
+      <c r="AR33" s="54"/>
       <c r="AS33" s="2">
         <v>13</v>
       </c>
@@ -4918,7 +4924,7 @@
       <c r="AV33" s="3">
         <v>16</v>
       </c>
-      <c r="AW33" s="57"/>
+      <c r="AW33" s="54"/>
       <c r="AX33" s="2">
         <v>13</v>
       </c>
@@ -4931,7 +4937,7 @@
       <c r="BA33" s="3">
         <v>16</v>
       </c>
-      <c r="BB33" s="57"/>
+      <c r="BB33" s="54"/>
       <c r="BC33" s="2">
         <v>13</v>
       </c>
@@ -4944,7 +4950,7 @@
       <c r="BF33" s="3">
         <v>16</v>
       </c>
-      <c r="BG33" s="57"/>
+      <c r="BG33" s="54"/>
       <c r="BH33" s="2">
         <v>13</v>
       </c>
@@ -4959,7 +4965,7 @@
       </c>
     </row>
     <row r="34" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J34" s="58"/>
+      <c r="J34" s="55"/>
       <c r="K34" s="47">
         <v>17</v>
       </c>
@@ -4972,7 +4978,7 @@
       <c r="N34" s="48">
         <v>20</v>
       </c>
-      <c r="O34" s="58"/>
+      <c r="O34" s="55"/>
       <c r="P34" s="47">
         <v>17</v>
       </c>
@@ -4985,8 +4991,8 @@
       <c r="S34" s="48">
         <v>20</v>
       </c>
-      <c r="X34" s="58"/>
-      <c r="Y34" s="4">
+      <c r="X34" s="55"/>
+      <c r="Y34" s="47">
         <v>17</v>
       </c>
       <c r="Z34" s="5">
@@ -4995,10 +5001,10 @@
       <c r="AA34" s="5">
         <v>19</v>
       </c>
-      <c r="AB34" s="6">
+      <c r="AB34" s="48">
         <v>20</v>
       </c>
-      <c r="AC34" s="58"/>
+      <c r="AC34" s="55"/>
       <c r="AD34" s="4">
         <v>17</v>
       </c>
@@ -5011,7 +5017,7 @@
       <c r="AG34" s="6">
         <v>20</v>
       </c>
-      <c r="AH34" s="58"/>
+      <c r="AH34" s="55"/>
       <c r="AI34" s="4">
         <v>17</v>
       </c>
@@ -5024,7 +5030,7 @@
       <c r="AL34" s="6">
         <v>20</v>
       </c>
-      <c r="AM34" s="58"/>
+      <c r="AM34" s="55"/>
       <c r="AN34" s="4">
         <v>17</v>
       </c>
@@ -5037,7 +5043,7 @@
       <c r="AQ34" s="6">
         <v>20</v>
       </c>
-      <c r="AR34" s="58"/>
+      <c r="AR34" s="55"/>
       <c r="AS34" s="4">
         <v>17</v>
       </c>
@@ -5050,7 +5056,7 @@
       <c r="AV34" s="6">
         <v>20</v>
       </c>
-      <c r="AW34" s="58"/>
+      <c r="AW34" s="55"/>
       <c r="AX34" s="4">
         <v>17</v>
       </c>
@@ -5063,7 +5069,7 @@
       <c r="BA34" s="6">
         <v>20</v>
       </c>
-      <c r="BB34" s="58"/>
+      <c r="BB34" s="55"/>
       <c r="BC34" s="4">
         <v>17</v>
       </c>
@@ -5076,7 +5082,7 @@
       <c r="BF34" s="6">
         <v>20</v>
       </c>
-      <c r="BG34" s="58"/>
+      <c r="BG34" s="55"/>
       <c r="BH34" s="4">
         <v>17</v>
       </c>
@@ -5091,7 +5097,7 @@
       </c>
     </row>
     <row r="35" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J35" s="87">
+      <c r="J35" s="88">
         <v>5</v>
       </c>
       <c r="K35" s="44">
@@ -5106,7 +5112,7 @@
       <c r="N35" s="50">
         <v>4</v>
       </c>
-      <c r="O35" s="87">
+      <c r="O35" s="88">
         <v>5</v>
       </c>
       <c r="P35" s="44">
@@ -5121,10 +5127,10 @@
       <c r="S35" s="50">
         <v>4</v>
       </c>
-      <c r="X35" s="56">
-        <v>5</v>
-      </c>
-      <c r="Y35" s="7">
+      <c r="X35" s="73">
+        <v>5</v>
+      </c>
+      <c r="Y35" s="44">
         <v>1</v>
       </c>
       <c r="Z35" s="8">
@@ -5133,10 +5139,10 @@
       <c r="AA35" s="8">
         <v>3</v>
       </c>
-      <c r="AB35" s="9">
-        <v>4</v>
-      </c>
-      <c r="AC35" s="56">
+      <c r="AB35" s="50">
+        <v>4</v>
+      </c>
+      <c r="AC35" s="53">
         <v>5</v>
       </c>
       <c r="AD35" s="7">
@@ -5151,7 +5157,7 @@
       <c r="AG35" s="9">
         <v>4</v>
       </c>
-      <c r="AH35" s="56">
+      <c r="AH35" s="53">
         <v>5</v>
       </c>
       <c r="AI35" s="7">
@@ -5166,7 +5172,7 @@
       <c r="AL35" s="9">
         <v>4</v>
       </c>
-      <c r="AM35" s="56">
+      <c r="AM35" s="53">
         <v>5</v>
       </c>
       <c r="AN35" s="7">
@@ -5181,7 +5187,7 @@
       <c r="AQ35" s="9">
         <v>4</v>
       </c>
-      <c r="AR35" s="56">
+      <c r="AR35" s="53">
         <v>5</v>
       </c>
       <c r="AS35" s="7">
@@ -5196,7 +5202,7 @@
       <c r="AV35" s="9">
         <v>4</v>
       </c>
-      <c r="AW35" s="56">
+      <c r="AW35" s="53">
         <v>5</v>
       </c>
       <c r="AX35" s="7">
@@ -5211,7 +5217,7 @@
       <c r="BA35" s="9">
         <v>4</v>
       </c>
-      <c r="BB35" s="56">
+      <c r="BB35" s="53">
         <v>5</v>
       </c>
       <c r="BC35" s="7">
@@ -5226,7 +5232,7 @@
       <c r="BF35" s="9">
         <v>4</v>
       </c>
-      <c r="BG35" s="56">
+      <c r="BG35" s="53">
         <v>5</v>
       </c>
       <c r="BH35" s="7">
@@ -5243,7 +5249,7 @@
       </c>
     </row>
     <row r="36" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J36" s="57"/>
+      <c r="J36" s="54"/>
       <c r="K36" s="42">
         <v>5</v>
       </c>
@@ -5256,7 +5262,7 @@
       <c r="N36" s="43">
         <v>8</v>
       </c>
-      <c r="O36" s="57"/>
+      <c r="O36" s="54"/>
       <c r="P36" s="42">
         <v>5</v>
       </c>
@@ -5269,8 +5275,8 @@
       <c r="S36" s="43">
         <v>8</v>
       </c>
-      <c r="X36" s="57"/>
-      <c r="Y36" s="2">
+      <c r="X36" s="54"/>
+      <c r="Y36" s="42">
         <v>5</v>
       </c>
       <c r="Z36" s="1">
@@ -5279,10 +5285,10 @@
       <c r="AA36" s="1">
         <v>7</v>
       </c>
-      <c r="AB36" s="3">
+      <c r="AB36" s="43">
         <v>8</v>
       </c>
-      <c r="AC36" s="57"/>
+      <c r="AC36" s="54"/>
       <c r="AD36" s="2">
         <v>5</v>
       </c>
@@ -5295,7 +5301,7 @@
       <c r="AG36" s="3">
         <v>8</v>
       </c>
-      <c r="AH36" s="57"/>
+      <c r="AH36" s="54"/>
       <c r="AI36" s="2">
         <v>5</v>
       </c>
@@ -5308,7 +5314,7 @@
       <c r="AL36" s="3">
         <v>8</v>
       </c>
-      <c r="AM36" s="57"/>
+      <c r="AM36" s="54"/>
       <c r="AN36" s="2">
         <v>5</v>
       </c>
@@ -5321,7 +5327,7 @@
       <c r="AQ36" s="3">
         <v>8</v>
       </c>
-      <c r="AR36" s="57"/>
+      <c r="AR36" s="54"/>
       <c r="AS36" s="2">
         <v>5</v>
       </c>
@@ -5334,7 +5340,7 @@
       <c r="AV36" s="3">
         <v>8</v>
       </c>
-      <c r="AW36" s="57"/>
+      <c r="AW36" s="54"/>
       <c r="AX36" s="2">
         <v>5</v>
       </c>
@@ -5347,7 +5353,7 @@
       <c r="BA36" s="3">
         <v>8</v>
       </c>
-      <c r="BB36" s="57"/>
+      <c r="BB36" s="54"/>
       <c r="BC36" s="2">
         <v>5</v>
       </c>
@@ -5360,7 +5366,7 @@
       <c r="BF36" s="3">
         <v>8</v>
       </c>
-      <c r="BG36" s="57"/>
+      <c r="BG36" s="54"/>
       <c r="BH36" s="2">
         <v>5</v>
       </c>
@@ -5375,7 +5381,7 @@
       </c>
     </row>
     <row r="37" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J37" s="57"/>
+      <c r="J37" s="54"/>
       <c r="K37" s="42">
         <v>9</v>
       </c>
@@ -5388,7 +5394,7 @@
       <c r="N37" s="43">
         <v>12</v>
       </c>
-      <c r="O37" s="57"/>
+      <c r="O37" s="54"/>
       <c r="P37" s="42">
         <v>9</v>
       </c>
@@ -5401,8 +5407,8 @@
       <c r="S37" s="43">
         <v>12</v>
       </c>
-      <c r="X37" s="57"/>
-      <c r="Y37" s="2">
+      <c r="X37" s="54"/>
+      <c r="Y37" s="42">
         <v>9</v>
       </c>
       <c r="Z37" s="1">
@@ -5411,10 +5417,10 @@
       <c r="AA37" s="1">
         <v>11</v>
       </c>
-      <c r="AB37" s="3">
+      <c r="AB37" s="43">
         <v>12</v>
       </c>
-      <c r="AC37" s="57"/>
+      <c r="AC37" s="54"/>
       <c r="AD37" s="2">
         <v>9</v>
       </c>
@@ -5427,7 +5433,7 @@
       <c r="AG37" s="3">
         <v>12</v>
       </c>
-      <c r="AH37" s="57"/>
+      <c r="AH37" s="54"/>
       <c r="AI37" s="2">
         <v>9</v>
       </c>
@@ -5440,7 +5446,7 @@
       <c r="AL37" s="3">
         <v>12</v>
       </c>
-      <c r="AM37" s="57"/>
+      <c r="AM37" s="54"/>
       <c r="AN37" s="2">
         <v>9</v>
       </c>
@@ -5453,7 +5459,7 @@
       <c r="AQ37" s="3">
         <v>12</v>
       </c>
-      <c r="AR37" s="57"/>
+      <c r="AR37" s="54"/>
       <c r="AS37" s="2">
         <v>9</v>
       </c>
@@ -5466,7 +5472,7 @@
       <c r="AV37" s="3">
         <v>12</v>
       </c>
-      <c r="AW37" s="57"/>
+      <c r="AW37" s="54"/>
       <c r="AX37" s="2">
         <v>9</v>
       </c>
@@ -5479,7 +5485,7 @@
       <c r="BA37" s="3">
         <v>12</v>
       </c>
-      <c r="BB37" s="57"/>
+      <c r="BB37" s="54"/>
       <c r="BC37" s="2">
         <v>9</v>
       </c>
@@ -5492,7 +5498,7 @@
       <c r="BF37" s="3">
         <v>12</v>
       </c>
-      <c r="BG37" s="57"/>
+      <c r="BG37" s="54"/>
       <c r="BH37" s="2">
         <v>9</v>
       </c>
@@ -5507,7 +5513,7 @@
       </c>
     </row>
     <row r="38" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J38" s="57"/>
+      <c r="J38" s="54"/>
       <c r="K38" s="42">
         <v>13</v>
       </c>
@@ -5520,7 +5526,7 @@
       <c r="N38" s="43">
         <v>16</v>
       </c>
-      <c r="O38" s="57"/>
+      <c r="O38" s="54"/>
       <c r="P38" s="42">
         <v>13</v>
       </c>
@@ -5533,8 +5539,8 @@
       <c r="S38" s="43">
         <v>16</v>
       </c>
-      <c r="X38" s="57"/>
-      <c r="Y38" s="2">
+      <c r="X38" s="54"/>
+      <c r="Y38" s="42">
         <v>13</v>
       </c>
       <c r="Z38" s="1">
@@ -5543,10 +5549,10 @@
       <c r="AA38" s="1">
         <v>15</v>
       </c>
-      <c r="AB38" s="3">
+      <c r="AB38" s="43">
         <v>16</v>
       </c>
-      <c r="AC38" s="57"/>
+      <c r="AC38" s="54"/>
       <c r="AD38" s="2">
         <v>13</v>
       </c>
@@ -5559,7 +5565,7 @@
       <c r="AG38" s="3">
         <v>16</v>
       </c>
-      <c r="AH38" s="57"/>
+      <c r="AH38" s="54"/>
       <c r="AI38" s="2">
         <v>13</v>
       </c>
@@ -5572,7 +5578,7 @@
       <c r="AL38" s="3">
         <v>16</v>
       </c>
-      <c r="AM38" s="57"/>
+      <c r="AM38" s="54"/>
       <c r="AN38" s="2">
         <v>13</v>
       </c>
@@ -5585,7 +5591,7 @@
       <c r="AQ38" s="3">
         <v>16</v>
       </c>
-      <c r="AR38" s="57"/>
+      <c r="AR38" s="54"/>
       <c r="AS38" s="2">
         <v>13</v>
       </c>
@@ -5598,7 +5604,7 @@
       <c r="AV38" s="3">
         <v>16</v>
       </c>
-      <c r="AW38" s="57"/>
+      <c r="AW38" s="54"/>
       <c r="AX38" s="2">
         <v>13</v>
       </c>
@@ -5611,7 +5617,7 @@
       <c r="BA38" s="3">
         <v>16</v>
       </c>
-      <c r="BB38" s="57"/>
+      <c r="BB38" s="54"/>
       <c r="BC38" s="2">
         <v>13</v>
       </c>
@@ -5624,7 +5630,7 @@
       <c r="BF38" s="3">
         <v>16</v>
       </c>
-      <c r="BG38" s="57"/>
+      <c r="BG38" s="54"/>
       <c r="BH38" s="2">
         <v>13</v>
       </c>
@@ -5639,7 +5645,7 @@
       </c>
     </row>
     <row r="39" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J39" s="58"/>
+      <c r="J39" s="55"/>
       <c r="K39" s="47">
         <v>17</v>
       </c>
@@ -5652,7 +5658,7 @@
       <c r="N39" s="48">
         <v>20</v>
       </c>
-      <c r="O39" s="58"/>
+      <c r="O39" s="55"/>
       <c r="P39" s="47">
         <v>17</v>
       </c>
@@ -5665,8 +5671,8 @@
       <c r="S39" s="48">
         <v>20</v>
       </c>
-      <c r="X39" s="58"/>
-      <c r="Y39" s="4">
+      <c r="X39" s="55"/>
+      <c r="Y39" s="47">
         <v>17</v>
       </c>
       <c r="Z39" s="5">
@@ -5675,10 +5681,10 @@
       <c r="AA39" s="5">
         <v>19</v>
       </c>
-      <c r="AB39" s="6">
+      <c r="AB39" s="48">
         <v>20</v>
       </c>
-      <c r="AC39" s="58"/>
+      <c r="AC39" s="55"/>
       <c r="AD39" s="4">
         <v>17</v>
       </c>
@@ -5691,7 +5697,7 @@
       <c r="AG39" s="6">
         <v>20</v>
       </c>
-      <c r="AH39" s="58"/>
+      <c r="AH39" s="55"/>
       <c r="AI39" s="4">
         <v>17</v>
       </c>
@@ -5704,7 +5710,7 @@
       <c r="AL39" s="6">
         <v>20</v>
       </c>
-      <c r="AM39" s="58"/>
+      <c r="AM39" s="55"/>
       <c r="AN39" s="4">
         <v>17</v>
       </c>
@@ -5717,7 +5723,7 @@
       <c r="AQ39" s="6">
         <v>20</v>
       </c>
-      <c r="AR39" s="58"/>
+      <c r="AR39" s="55"/>
       <c r="AS39" s="4">
         <v>17</v>
       </c>
@@ -5730,7 +5736,7 @@
       <c r="AV39" s="6">
         <v>20</v>
       </c>
-      <c r="AW39" s="58"/>
+      <c r="AW39" s="55"/>
       <c r="AX39" s="4">
         <v>17</v>
       </c>
@@ -5743,7 +5749,7 @@
       <c r="BA39" s="6">
         <v>20</v>
       </c>
-      <c r="BB39" s="58"/>
+      <c r="BB39" s="55"/>
       <c r="BC39" s="4">
         <v>17</v>
       </c>
@@ -5756,7 +5762,7 @@
       <c r="BF39" s="6">
         <v>20</v>
       </c>
-      <c r="BG39" s="58"/>
+      <c r="BG39" s="55"/>
       <c r="BH39" s="4">
         <v>17</v>
       </c>
@@ -5771,7 +5777,7 @@
       </c>
     </row>
     <row r="40" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J40" s="110">
+      <c r="J40" s="111">
         <v>6</v>
       </c>
       <c r="K40" s="42">
@@ -5786,7 +5792,7 @@
       <c r="N40" s="43">
         <v>4</v>
       </c>
-      <c r="O40" s="110">
+      <c r="O40" s="111">
         <v>6</v>
       </c>
       <c r="P40" s="42">
@@ -5801,10 +5807,10 @@
       <c r="S40" s="43">
         <v>4</v>
       </c>
-      <c r="X40" s="79">
-        <v>6</v>
-      </c>
-      <c r="Y40" s="2">
+      <c r="X40" s="114">
+        <v>6</v>
+      </c>
+      <c r="Y40" s="42">
         <v>1</v>
       </c>
       <c r="Z40" s="1">
@@ -5813,10 +5819,10 @@
       <c r="AA40" s="1">
         <v>3</v>
       </c>
-      <c r="AB40" s="3">
-        <v>4</v>
-      </c>
-      <c r="AC40" s="56">
+      <c r="AB40" s="43">
+        <v>4</v>
+      </c>
+      <c r="AC40" s="53">
         <v>6</v>
       </c>
       <c r="AD40" s="7">
@@ -5831,7 +5837,7 @@
       <c r="AG40" s="9">
         <v>4</v>
       </c>
-      <c r="AH40" s="56">
+      <c r="AH40" s="53">
         <v>6</v>
       </c>
       <c r="AI40" s="7">
@@ -5846,7 +5852,7 @@
       <c r="AL40" s="9">
         <v>4</v>
       </c>
-      <c r="AM40" s="79">
+      <c r="AM40" s="80">
         <v>6</v>
       </c>
       <c r="AN40" s="2">
@@ -5861,7 +5867,7 @@
       <c r="AQ40" s="3">
         <v>4</v>
       </c>
-      <c r="AR40" s="79">
+      <c r="AR40" s="80">
         <v>6</v>
       </c>
       <c r="AS40" s="2">
@@ -5876,7 +5882,7 @@
       <c r="AV40" s="3">
         <v>4</v>
       </c>
-      <c r="AW40" s="79">
+      <c r="AW40" s="80">
         <v>6</v>
       </c>
       <c r="AX40" s="2">
@@ -5891,7 +5897,7 @@
       <c r="BA40" s="3">
         <v>4</v>
       </c>
-      <c r="BB40" s="79">
+      <c r="BB40" s="80">
         <v>6</v>
       </c>
       <c r="BC40" s="2">
@@ -5906,7 +5912,7 @@
       <c r="BF40" s="3">
         <v>4</v>
       </c>
-      <c r="BG40" s="79">
+      <c r="BG40" s="80">
         <v>6</v>
       </c>
       <c r="BH40" s="2">
@@ -5923,7 +5929,7 @@
       </c>
     </row>
     <row r="41" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J41" s="57"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="42">
         <v>5</v>
       </c>
@@ -5936,7 +5942,7 @@
       <c r="N41" s="43">
         <v>8</v>
       </c>
-      <c r="O41" s="57"/>
+      <c r="O41" s="54"/>
       <c r="P41" s="42">
         <v>5</v>
       </c>
@@ -5949,8 +5955,8 @@
       <c r="S41" s="43">
         <v>8</v>
       </c>
-      <c r="X41" s="57"/>
-      <c r="Y41" s="2">
+      <c r="X41" s="54"/>
+      <c r="Y41" s="42">
         <v>5</v>
       </c>
       <c r="Z41" s="1">
@@ -5959,10 +5965,10 @@
       <c r="AA41" s="1">
         <v>7</v>
       </c>
-      <c r="AB41" s="3">
+      <c r="AB41" s="43">
         <v>8</v>
       </c>
-      <c r="AC41" s="57"/>
+      <c r="AC41" s="54"/>
       <c r="AD41" s="2">
         <v>5</v>
       </c>
@@ -5975,7 +5981,7 @@
       <c r="AG41" s="3">
         <v>8</v>
       </c>
-      <c r="AH41" s="57"/>
+      <c r="AH41" s="54"/>
       <c r="AI41" s="2">
         <v>5</v>
       </c>
@@ -5988,7 +5994,7 @@
       <c r="AL41" s="3">
         <v>8</v>
       </c>
-      <c r="AM41" s="57"/>
+      <c r="AM41" s="54"/>
       <c r="AN41" s="2">
         <v>5</v>
       </c>
@@ -6001,7 +6007,7 @@
       <c r="AQ41" s="3">
         <v>8</v>
       </c>
-      <c r="AR41" s="57"/>
+      <c r="AR41" s="54"/>
       <c r="AS41" s="2">
         <v>5</v>
       </c>
@@ -6014,7 +6020,7 @@
       <c r="AV41" s="3">
         <v>8</v>
       </c>
-      <c r="AW41" s="57"/>
+      <c r="AW41" s="54"/>
       <c r="AX41" s="2">
         <v>5</v>
       </c>
@@ -6027,7 +6033,7 @@
       <c r="BA41" s="3">
         <v>8</v>
       </c>
-      <c r="BB41" s="57"/>
+      <c r="BB41" s="54"/>
       <c r="BC41" s="2">
         <v>5</v>
       </c>
@@ -6040,7 +6046,7 @@
       <c r="BF41" s="3">
         <v>8</v>
       </c>
-      <c r="BG41" s="57"/>
+      <c r="BG41" s="54"/>
       <c r="BH41" s="2">
         <v>5</v>
       </c>
@@ -6055,7 +6061,7 @@
       </c>
     </row>
     <row r="42" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J42" s="57"/>
+      <c r="J42" s="54"/>
       <c r="K42" s="42">
         <v>9</v>
       </c>
@@ -6068,7 +6074,7 @@
       <c r="N42" s="43">
         <v>12</v>
       </c>
-      <c r="O42" s="57"/>
+      <c r="O42" s="54"/>
       <c r="P42" s="42">
         <v>9</v>
       </c>
@@ -6081,8 +6087,8 @@
       <c r="S42" s="43">
         <v>12</v>
       </c>
-      <c r="X42" s="57"/>
-      <c r="Y42" s="2">
+      <c r="X42" s="54"/>
+      <c r="Y42" s="42">
         <v>9</v>
       </c>
       <c r="Z42" s="1">
@@ -6091,10 +6097,10 @@
       <c r="AA42" s="1">
         <v>11</v>
       </c>
-      <c r="AB42" s="3">
+      <c r="AB42" s="43">
         <v>12</v>
       </c>
-      <c r="AC42" s="57"/>
+      <c r="AC42" s="54"/>
       <c r="AD42" s="2">
         <v>9</v>
       </c>
@@ -6107,7 +6113,7 @@
       <c r="AG42" s="3">
         <v>12</v>
       </c>
-      <c r="AH42" s="57"/>
+      <c r="AH42" s="54"/>
       <c r="AI42" s="2">
         <v>9</v>
       </c>
@@ -6120,7 +6126,7 @@
       <c r="AL42" s="3">
         <v>12</v>
       </c>
-      <c r="AM42" s="57"/>
+      <c r="AM42" s="54"/>
       <c r="AN42" s="2">
         <v>9</v>
       </c>
@@ -6133,7 +6139,7 @@
       <c r="AQ42" s="3">
         <v>12</v>
       </c>
-      <c r="AR42" s="57"/>
+      <c r="AR42" s="54"/>
       <c r="AS42" s="2">
         <v>9</v>
       </c>
@@ -6146,7 +6152,7 @@
       <c r="AV42" s="3">
         <v>12</v>
       </c>
-      <c r="AW42" s="57"/>
+      <c r="AW42" s="54"/>
       <c r="AX42" s="2">
         <v>9</v>
       </c>
@@ -6159,7 +6165,7 @@
       <c r="BA42" s="3">
         <v>12</v>
       </c>
-      <c r="BB42" s="57"/>
+      <c r="BB42" s="54"/>
       <c r="BC42" s="2">
         <v>9</v>
       </c>
@@ -6172,7 +6178,7 @@
       <c r="BF42" s="3">
         <v>12</v>
       </c>
-      <c r="BG42" s="57"/>
+      <c r="BG42" s="54"/>
       <c r="BH42" s="2">
         <v>9</v>
       </c>
@@ -6187,7 +6193,7 @@
       </c>
     </row>
     <row r="43" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="J43" s="57"/>
+      <c r="J43" s="54"/>
       <c r="K43" s="42">
         <v>13</v>
       </c>
@@ -6200,7 +6206,7 @@
       <c r="N43" s="43">
         <v>16</v>
       </c>
-      <c r="O43" s="57"/>
+      <c r="O43" s="54"/>
       <c r="P43" s="42">
         <v>13</v>
       </c>
@@ -6213,8 +6219,8 @@
       <c r="S43" s="43">
         <v>16</v>
       </c>
-      <c r="X43" s="57"/>
-      <c r="Y43" s="2">
+      <c r="X43" s="54"/>
+      <c r="Y43" s="42">
         <v>13</v>
       </c>
       <c r="Z43" s="1">
@@ -6223,10 +6229,10 @@
       <c r="AA43" s="1">
         <v>15</v>
       </c>
-      <c r="AB43" s="3">
+      <c r="AB43" s="43">
         <v>16</v>
       </c>
-      <c r="AC43" s="57"/>
+      <c r="AC43" s="54"/>
       <c r="AD43" s="2">
         <v>13</v>
       </c>
@@ -6239,7 +6245,7 @@
       <c r="AG43" s="3">
         <v>16</v>
       </c>
-      <c r="AH43" s="57"/>
+      <c r="AH43" s="54"/>
       <c r="AI43" s="2">
         <v>13</v>
       </c>
@@ -6252,7 +6258,7 @@
       <c r="AL43" s="3">
         <v>16</v>
       </c>
-      <c r="AM43" s="57"/>
+      <c r="AM43" s="54"/>
       <c r="AN43" s="2">
         <v>13</v>
       </c>
@@ -6265,7 +6271,7 @@
       <c r="AQ43" s="3">
         <v>16</v>
       </c>
-      <c r="AR43" s="57"/>
+      <c r="AR43" s="54"/>
       <c r="AS43" s="2">
         <v>13</v>
       </c>
@@ -6278,7 +6284,7 @@
       <c r="AV43" s="3">
         <v>16</v>
       </c>
-      <c r="AW43" s="57"/>
+      <c r="AW43" s="54"/>
       <c r="AX43" s="2">
         <v>13</v>
       </c>
@@ -6291,7 +6297,7 @@
       <c r="BA43" s="3">
         <v>16</v>
       </c>
-      <c r="BB43" s="57"/>
+      <c r="BB43" s="54"/>
       <c r="BC43" s="2">
         <v>13</v>
       </c>
@@ -6304,7 +6310,7 @@
       <c r="BF43" s="3">
         <v>16</v>
       </c>
-      <c r="BG43" s="57"/>
+      <c r="BG43" s="54"/>
       <c r="BH43" s="2">
         <v>13</v>
       </c>
@@ -6319,7 +6325,7 @@
       </c>
     </row>
     <row r="44" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J44" s="57"/>
+      <c r="J44" s="54"/>
       <c r="K44" s="42">
         <v>17</v>
       </c>
@@ -6332,7 +6338,7 @@
       <c r="N44" s="43">
         <v>20</v>
       </c>
-      <c r="O44" s="57"/>
+      <c r="O44" s="54"/>
       <c r="P44" s="42">
         <v>17</v>
       </c>
@@ -6345,8 +6351,8 @@
       <c r="S44" s="43">
         <v>20</v>
       </c>
-      <c r="X44" s="57"/>
-      <c r="Y44" s="2">
+      <c r="X44" s="54"/>
+      <c r="Y44" s="42">
         <v>17</v>
       </c>
       <c r="Z44" s="1">
@@ -6355,10 +6361,10 @@
       <c r="AA44" s="1">
         <v>19</v>
       </c>
-      <c r="AB44" s="3">
+      <c r="AB44" s="43">
         <v>20</v>
       </c>
-      <c r="AC44" s="58"/>
+      <c r="AC44" s="55"/>
       <c r="AD44" s="4">
         <v>17</v>
       </c>
@@ -6371,7 +6377,7 @@
       <c r="AG44" s="6">
         <v>20</v>
       </c>
-      <c r="AH44" s="58"/>
+      <c r="AH44" s="55"/>
       <c r="AI44" s="4">
         <v>17</v>
       </c>
@@ -6384,7 +6390,7 @@
       <c r="AL44" s="6">
         <v>20</v>
       </c>
-      <c r="AM44" s="57"/>
+      <c r="AM44" s="54"/>
       <c r="AN44" s="2">
         <v>17</v>
       </c>
@@ -6397,7 +6403,7 @@
       <c r="AQ44" s="3">
         <v>20</v>
       </c>
-      <c r="AR44" s="57"/>
+      <c r="AR44" s="54"/>
       <c r="AS44" s="2">
         <v>17</v>
       </c>
@@ -6410,7 +6416,7 @@
       <c r="AV44" s="3">
         <v>20</v>
       </c>
-      <c r="AW44" s="57"/>
+      <c r="AW44" s="54"/>
       <c r="AX44" s="2">
         <v>17</v>
       </c>
@@ -6423,7 +6429,7 @@
       <c r="BA44" s="3">
         <v>20</v>
       </c>
-      <c r="BB44" s="57"/>
+      <c r="BB44" s="54"/>
       <c r="BC44" s="2">
         <v>17</v>
       </c>
@@ -6436,7 +6442,7 @@
       <c r="BF44" s="3">
         <v>20</v>
       </c>
-      <c r="BG44" s="57"/>
+      <c r="BG44" s="54"/>
       <c r="BH44" s="2">
         <v>17</v>
       </c>
@@ -6451,12 +6457,12 @@
       </c>
     </row>
     <row r="45" spans="1:63" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="121" t="s">
+      <c r="A45" s="123" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="103"/>
+      <c r="B45" s="104"/>
       <c r="C45" s="15"/>
-      <c r="D45" s="80" t="s">
+      <c r="D45" s="81" t="s">
         <v>51</v>
       </c>
       <c r="E45" s="65"/>
@@ -6466,14 +6472,14 @@
       <c r="I45" s="17"/>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
-      <c r="L45" s="86" t="s">
+      <c r="L45" s="87" t="s">
         <v>52</v>
       </c>
       <c r="M45" s="65"/>
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
       <c r="P45" s="16"/>
-      <c r="Q45" s="114" t="s">
+      <c r="Q45" s="116" t="s">
         <v>53</v>
       </c>
       <c r="R45" s="70"/>
@@ -6524,10 +6530,10 @@
       <c r="BK45" s="29"/>
     </row>
     <row r="46" spans="1:63" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="81"/>
-      <c r="E46" s="78"/>
-      <c r="L46" s="81"/>
-      <c r="M46" s="78"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="79"/>
+      <c r="L46" s="82"/>
+      <c r="M46" s="79"/>
     </row>
     <row r="47" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D47" s="66"/>
@@ -6565,6 +6571,10 @@
     </row>
   </sheetData>
   <mergeCells count="166">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="BH14:BK14"/>
+    <mergeCell ref="BG35:BG39"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="J15:J19"/>
@@ -6586,8 +6596,6 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="T15:V15"/>
     <mergeCell ref="Y14:AB14"/>
-    <mergeCell ref="O8:S8"/>
-    <mergeCell ref="BG35:BG39"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H16:I16"/>
@@ -6636,10 +6644,6 @@
     <mergeCell ref="O13:S13"/>
     <mergeCell ref="O7:S7"/>
     <mergeCell ref="J30:J34"/>
-    <mergeCell ref="BG7:BK7"/>
-    <mergeCell ref="BB30:BB34"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="AH20:AH24"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="BB20:BB24"/>
     <mergeCell ref="O35:O39"/>
@@ -6648,10 +6652,11 @@
     <mergeCell ref="O25:O29"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="BB13:BF13"/>
+    <mergeCell ref="AR40:AR44"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="BB7:BF7"/>
+    <mergeCell ref="X15:X19"/>
     <mergeCell ref="AM35:AM39"/>
-    <mergeCell ref="X15:X19"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F18:G18"/>
@@ -6660,6 +6665,9 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="O40:O44"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="AD14:AG14"/>
     <mergeCell ref="D7:E7"/>
@@ -6672,10 +6680,9 @@
     <mergeCell ref="T14:V14"/>
     <mergeCell ref="AM7:AQ7"/>
     <mergeCell ref="AM40:AM44"/>
-    <mergeCell ref="AR40:AR44"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="O40:O44"/>
+    <mergeCell ref="BB30:BB34"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="AH20:AH24"/>
     <mergeCell ref="AH9:AL10"/>
     <mergeCell ref="AR15:AR19"/>
     <mergeCell ref="J20:J24"/>
@@ -6684,10 +6691,11 @@
     <mergeCell ref="AW7:BA7"/>
     <mergeCell ref="AH30:AH34"/>
     <mergeCell ref="AR30:AR34"/>
+    <mergeCell ref="X20:X24"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="AS14:AV14"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="AW13:BA13"/>
+    <mergeCell ref="AM9:BK10"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="AW40:AW44"/>
     <mergeCell ref="AM15:AM19"/>
@@ -6695,36 +6703,34 @@
     <mergeCell ref="D45:E47"/>
     <mergeCell ref="AR20:AR24"/>
     <mergeCell ref="AH25:AH29"/>
+    <mergeCell ref="BG7:BK7"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="X20:X24"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="AX14:BA14"/>
     <mergeCell ref="A11:C12"/>
     <mergeCell ref="AM25:AM29"/>
+    <mergeCell ref="BG25:BG29"/>
     <mergeCell ref="T7:V7"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="X40:X44"/>
     <mergeCell ref="T16:V16"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="BG13:BK13"/>
     <mergeCell ref="BG30:BG34"/>
     <mergeCell ref="AM20:AM24"/>
     <mergeCell ref="X11:BK12"/>
     <mergeCell ref="BB25:BB29"/>
     <mergeCell ref="D11:G12"/>
     <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="AH8:AL8"/>
     <mergeCell ref="AI14:AL14"/>
+    <mergeCell ref="X35:X39"/>
     <mergeCell ref="J11:S12"/>
-    <mergeCell ref="X35:X39"/>
-    <mergeCell ref="AH8:AL8"/>
-    <mergeCell ref="AM9:BK10"/>
-    <mergeCell ref="BG25:BG29"/>
-    <mergeCell ref="BG13:BK13"/>
+    <mergeCell ref="AW13:BA13"/>
     <mergeCell ref="BC14:BF14"/>
-    <mergeCell ref="BH14:BK14"/>
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="AH40:AH44"/>
     <mergeCell ref="K14:N14"/>
-    <mergeCell ref="AH40:AH44"/>
     <mergeCell ref="AR7:AV7"/>
     <mergeCell ref="AM30:AM34"/>
     <mergeCell ref="F16:G16"/>

</xml_diff>